<commit_message>
Bugfix and minor code change
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES005.xlsx
+++ b/apps/es/resources/screen/ES005.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="433">
   <si>
     <t>Do not modify this column</t>
   </si>
@@ -553,6 +553,18 @@
     <t>Settle Date To</t>
   </si>
   <si>
+    <t>schExpenseCtgField</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>schExpensePrjField</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
     <t>schExpenseDscField</t>
   </si>
   <si>
@@ -709,9 +721,6 @@
     <t>catField</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>cat.cat</t>
   </si>
   <si>
@@ -764,9 +773,6 @@
   </si>
   <si>
     <t>prjField</t>
-  </si>
-  <si>
-    <t>Project</t>
   </si>
   <si>
     <t>prj_nm</t>
@@ -1346,7 +1352,7 @@
     <t>One tailor made javascript for each layout</t>
   </si>
   <si>
-    <t>20250512160900</t>
+    <t>20250516135000</t>
   </si>
 </sst>
 </file>
@@ -1892,7 +1898,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T204"/>
+  <dimension ref="A1:T206"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -2092,7 +2098,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>37</v>
@@ -3207,7 +3213,7 @@
         <v>170</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
@@ -3224,14 +3230,12 @@
       <c r="P64" s="11"/>
     </row>
     <row r="65" spans="3:16">
-      <c r="C65" s="11" t="s">
-        <v>98</v>
-      </c>
+      <c r="C65" s="11"/>
       <c r="D65" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -3239,12 +3243,10 @@
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
       <c r="K65" s="11" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L65" s="11"/>
-      <c r="M65" s="11" t="s">
-        <v>173</v>
-      </c>
+      <c r="M65" s="11"/>
       <c r="N65" s="11"/>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
@@ -3255,33 +3257,31 @@
         <v>174</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>176</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
       <c r="K66" s="11" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L66" s="11"/>
-      <c r="M66" s="11" t="s">
-        <v>177</v>
-      </c>
+      <c r="M66" s="11"/>
       <c r="N66" s="11"/>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
     <row r="67" spans="3:16">
-      <c r="C67" s="11"/>
+      <c r="C67" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="D67" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
@@ -3289,11 +3289,11 @@
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
       <c r="K67" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L67" s="11"/>
       <c r="M67" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N67" s="11"/>
       <c r="O67" s="11"/>
@@ -3302,24 +3302,24 @@
     <row r="68" spans="3:16">
       <c r="C68" s="11"/>
       <c r="D68" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
       <c r="K68" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L68" s="11"/>
       <c r="M68" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N68" s="11"/>
       <c r="O68" s="11"/>
@@ -3328,10 +3328,10 @@
     <row r="69" spans="3:16">
       <c r="C69" s="11"/>
       <c r="D69" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
@@ -3339,11 +3339,11 @@
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
       <c r="K69" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L69" s="11"/>
       <c r="M69" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N69" s="11"/>
       <c r="O69" s="11"/>
@@ -3352,22 +3352,24 @@
     <row r="70" spans="3:16">
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>187</v>
-      </c>
       <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
+      <c r="G70" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L70" s="11"/>
       <c r="M70" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N70" s="11"/>
       <c r="O70" s="11"/>
@@ -3376,10 +3378,10 @@
     <row r="71" spans="3:16">
       <c r="C71" s="11"/>
       <c r="D71" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>190</v>
+        <v>11</v>
       </c>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
@@ -3387,13 +3389,11 @@
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L71" s="11" t="s">
-        <v>191</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L71" s="11"/>
       <c r="M71" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N71" s="11"/>
       <c r="O71" s="11"/>
@@ -3402,10 +3402,10 @@
     <row r="72" spans="3:16">
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
@@ -3413,11 +3413,11 @@
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L72" s="11"/>
       <c r="M72" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N72" s="11"/>
       <c r="O72" s="11"/>
@@ -3426,10 +3426,10 @@
     <row r="73" spans="3:16">
       <c r="C73" s="11"/>
       <c r="D73" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
@@ -3437,11 +3437,13 @@
       <c r="I73" s="11"/>
       <c r="J73" s="11"/>
       <c r="K73" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L73" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="L73" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="M73" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N73" s="11"/>
       <c r="O73" s="11"/>
@@ -3450,10 +3452,10 @@
     <row r="74" spans="3:16">
       <c r="C74" s="11"/>
       <c r="D74" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
@@ -3461,13 +3463,11 @@
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
       <c r="K74" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L74" s="11" t="s">
-        <v>191</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L74" s="11"/>
       <c r="M74" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N74" s="11"/>
       <c r="O74" s="11"/>
@@ -3476,10 +3476,10 @@
     <row r="75" spans="3:16">
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
@@ -3487,11 +3487,11 @@
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L75" s="11"/>
       <c r="M75" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N75" s="11"/>
       <c r="O75" s="11"/>
@@ -3500,10 +3500,10 @@
     <row r="76" spans="3:16">
       <c r="C76" s="11"/>
       <c r="D76" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -3511,11 +3511,13 @@
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L76" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="L76" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="M76" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N76" s="11"/>
       <c r="O76" s="11"/>
@@ -3524,10 +3526,10 @@
     <row r="77" spans="3:16">
       <c r="C77" s="11"/>
       <c r="D77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
@@ -3535,11 +3537,11 @@
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L77" s="11"/>
       <c r="M77" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N77" s="11"/>
       <c r="O77" s="11"/>
@@ -3548,36 +3550,34 @@
     <row r="78" spans="3:16">
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="E78" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>191</v>
+      </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="L78" s="11"/>
       <c r="M78" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="N78" s="11" t="s">
-        <v>212</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="N78" s="11"/>
       <c r="O78" s="11"/>
       <c r="P78" s="11"/>
     </row>
     <row r="79" spans="3:16">
-      <c r="C79" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="C79" s="11"/>
       <c r="D79" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
@@ -3585,11 +3585,11 @@
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
       <c r="K79" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L79" s="11"/>
       <c r="M79" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N79" s="11"/>
       <c r="O79" s="11"/>
@@ -3598,36 +3598,36 @@
     <row r="80" spans="3:16">
       <c r="C80" s="11"/>
       <c r="D80" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>217</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="E80" s="11"/>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
       <c r="K80" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L80" s="11" t="s">
-        <v>159</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="L80" s="11"/>
       <c r="M80" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="N80" s="11"/>
+        <v>215</v>
+      </c>
+      <c r="N80" s="11" t="s">
+        <v>216</v>
+      </c>
       <c r="O80" s="11"/>
       <c r="P80" s="11"/>
     </row>
     <row r="81" spans="3:16">
-      <c r="C81" s="11"/>
+      <c r="C81" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="D81" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
@@ -3635,11 +3635,11 @@
       <c r="I81" s="11"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L81" s="11"/>
       <c r="M81" s="11" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="N81" s="11"/>
       <c r="O81" s="11"/>
@@ -3648,10 +3648,10 @@
     <row r="82" spans="3:16">
       <c r="C82" s="11"/>
       <c r="D82" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E82" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>222</v>
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
@@ -3659,11 +3659,13 @@
       <c r="I82" s="11"/>
       <c r="J82" s="11"/>
       <c r="K82" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L82" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="L82" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="M82" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N82" s="11"/>
       <c r="O82" s="11"/>
@@ -3672,10 +3674,10 @@
     <row r="83" spans="3:16">
       <c r="C83" s="11"/>
       <c r="D83" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E83" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>225</v>
       </c>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
@@ -3683,11 +3685,11 @@
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L83" s="11"/>
       <c r="M83" s="11" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="N83" s="11"/>
       <c r="O83" s="11"/>
@@ -3696,10 +3698,10 @@
     <row r="84" spans="3:16">
       <c r="C84" s="11"/>
       <c r="D84" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>228</v>
+        <v>171</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -3707,13 +3709,11 @@
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
       <c r="K84" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L84" s="11" t="s">
-        <v>229</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L84" s="11"/>
       <c r="M84" s="11" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="N84" s="11"/>
       <c r="O84" s="11"/>
@@ -3722,10 +3722,10 @@
     <row r="85" spans="3:16">
       <c r="C85" s="11"/>
       <c r="D85" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
@@ -3733,13 +3733,11 @@
       <c r="I85" s="11"/>
       <c r="J85" s="11"/>
       <c r="K85" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L85" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L85" s="11"/>
+      <c r="M85" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="M85" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="N85" s="11"/>
       <c r="O85" s="11"/>
@@ -3748,10 +3746,10 @@
     <row r="86" spans="3:16">
       <c r="C86" s="11"/>
       <c r="D86" s="11" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -3759,11 +3757,13 @@
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
       <c r="K86" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L86" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="L86" s="11" t="s">
+        <v>232</v>
+      </c>
       <c r="M86" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="N86" s="11"/>
       <c r="O86" s="11"/>
@@ -3772,26 +3772,24 @@
     <row r="87" spans="3:16">
       <c r="C87" s="11"/>
       <c r="D87" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>238</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="F87" s="11"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
       <c r="K87" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L87" s="11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="M87" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="N87" s="11"/>
       <c r="O87" s="11"/>
@@ -3800,10 +3798,10 @@
     <row r="88" spans="3:16">
       <c r="C88" s="11"/>
       <c r="D88" s="11" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
@@ -3811,11 +3809,11 @@
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>
       <c r="K88" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L88" s="11"/>
       <c r="M88" s="11" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N88" s="11"/>
       <c r="O88" s="11"/>
@@ -3824,114 +3822,116 @@
     <row r="89" spans="3:16">
       <c r="C89" s="11"/>
       <c r="D89" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
+        <v>240</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>241</v>
+      </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
       <c r="J89" s="11"/>
       <c r="K89" s="11" t="s">
-        <v>244</v>
+        <v>176</v>
       </c>
       <c r="L89" s="11" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="M89" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="N89" s="11" t="s">
-        <v>247</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="N89" s="11"/>
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
     <row r="90" spans="3:16">
       <c r="C90" s="11"/>
       <c r="D90" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E90" s="11"/>
+        <v>243</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>173</v>
+      </c>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
       <c r="J90" s="11"/>
       <c r="K90" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L90" s="11"/>
+      <c r="M90" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="L90" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="M90" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="N90" s="11" t="s">
-        <v>251</v>
-      </c>
+      <c r="N90" s="11"/>
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
     <row r="91" spans="3:16">
-      <c r="C91" s="11" t="s">
-        <v>108</v>
-      </c>
+      <c r="C91" s="11"/>
       <c r="D91" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>214</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
       <c r="J91" s="11"/>
       <c r="K91" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L91" s="11"/>
+        <v>246</v>
+      </c>
+      <c r="L91" s="11" t="s">
+        <v>247</v>
+      </c>
       <c r="M91" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="N91" s="11"/>
+        <v>248</v>
+      </c>
+      <c r="N91" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
     <row r="92" spans="3:16">
       <c r="C92" s="11"/>
       <c r="D92" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>217</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="E92" s="11"/>
       <c r="F92" s="11"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
       <c r="I92" s="11"/>
       <c r="J92" s="11"/>
       <c r="K92" s="11" t="s">
-        <v>172</v>
+        <v>246</v>
       </c>
       <c r="L92" s="11" t="s">
-        <v>159</v>
+        <v>251</v>
       </c>
       <c r="M92" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="N92" s="11"/>
+        <v>252</v>
+      </c>
+      <c r="N92" s="11" t="s">
+        <v>253</v>
+      </c>
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
     <row r="93" spans="3:16">
-      <c r="C93" s="11"/>
+      <c r="C93" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="D93" s="11" t="s">
         <v>254</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
@@ -3939,11 +3939,11 @@
       <c r="I93" s="11"/>
       <c r="J93" s="11"/>
       <c r="K93" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L93" s="11"/>
       <c r="M93" s="11" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="N93" s="11"/>
       <c r="O93" s="11"/>
@@ -3955,7 +3955,7 @@
         <v>255</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
@@ -3963,11 +3963,13 @@
       <c r="I94" s="11"/>
       <c r="J94" s="11"/>
       <c r="K94" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L94" s="11"/>
+        <v>176</v>
+      </c>
+      <c r="L94" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="M94" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N94" s="11"/>
       <c r="O94" s="11"/>
@@ -3979,7 +3981,7 @@
         <v>256</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
@@ -3987,11 +3989,11 @@
       <c r="I95" s="11"/>
       <c r="J95" s="11"/>
       <c r="K95" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L95" s="11"/>
       <c r="M95" s="11" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="N95" s="11"/>
       <c r="O95" s="11"/>
@@ -4000,10 +4002,10 @@
     <row r="96" spans="3:16">
       <c r="C96" s="11"/>
       <c r="D96" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>259</v>
+        <v>171</v>
       </c>
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
@@ -4011,11 +4013,11 @@
       <c r="I96" s="11"/>
       <c r="J96" s="11"/>
       <c r="K96" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L96" s="11"/>
       <c r="M96" s="11" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="N96" s="11"/>
       <c r="O96" s="11"/>
@@ -4024,10 +4026,10 @@
     <row r="97" spans="3:16">
       <c r="C97" s="11"/>
       <c r="D97" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
@@ -4035,11 +4037,11 @@
       <c r="I97" s="11"/>
       <c r="J97" s="11"/>
       <c r="K97" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L97" s="11"/>
       <c r="M97" s="11" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="N97" s="11"/>
       <c r="O97" s="11"/>
@@ -4048,10 +4050,10 @@
     <row r="98" spans="3:16">
       <c r="C98" s="11"/>
       <c r="D98" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F98" s="11"/>
       <c r="G98" s="11"/>
@@ -4059,11 +4061,11 @@
       <c r="I98" s="11"/>
       <c r="J98" s="11"/>
       <c r="K98" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L98" s="11"/>
       <c r="M98" s="11" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="N98" s="11"/>
       <c r="O98" s="11"/>
@@ -4072,10 +4074,10 @@
     <row r="99" spans="3:16">
       <c r="C99" s="11"/>
       <c r="D99" s="11" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
@@ -4083,11 +4085,11 @@
       <c r="I99" s="11"/>
       <c r="J99" s="11"/>
       <c r="K99" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L99" s="11"/>
       <c r="M99" s="11" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="N99" s="11"/>
       <c r="O99" s="11"/>
@@ -4096,156 +4098,152 @@
     <row r="100" spans="3:16">
       <c r="C100" s="11"/>
       <c r="D100" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E100" s="11"/>
+        <v>265</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>266</v>
+      </c>
       <c r="F100" s="11"/>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
       <c r="I100" s="11"/>
       <c r="J100" s="11"/>
       <c r="K100" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="L100" s="11" t="s">
-        <v>245</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L100" s="11"/>
       <c r="M100" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="N100" s="11" t="s">
-        <v>268</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="N100" s="11"/>
       <c r="O100" s="11"/>
       <c r="P100" s="11"/>
     </row>
     <row r="101" spans="3:16">
       <c r="C101" s="11"/>
       <c r="D101" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="E101" s="11"/>
+        <v>268</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>173</v>
+      </c>
       <c r="F101" s="11"/>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>
       <c r="J101" s="11"/>
       <c r="K101" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L101" s="11"/>
+      <c r="M101" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="L101" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="M101" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="N101" s="11" t="s">
-        <v>271</v>
-      </c>
+      <c r="N101" s="11"/>
       <c r="O101" s="11"/>
       <c r="P101" s="11"/>
     </row>
     <row r="102" spans="3:16">
-      <c r="C102" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11" t="s">
-        <v>141</v>
-      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E102" s="11"/>
       <c r="F102" s="11"/>
       <c r="G102" s="11"/>
-      <c r="H102" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H102" s="11"/>
       <c r="I102" s="11"/>
       <c r="J102" s="11"/>
       <c r="K102" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L102" s="11"/>
+        <v>246</v>
+      </c>
+      <c r="L102" s="11" t="s">
+        <v>247</v>
+      </c>
       <c r="M102" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="N102" s="11"/>
+        <v>248</v>
+      </c>
+      <c r="N102" s="11" t="s">
+        <v>270</v>
+      </c>
       <c r="O102" s="11"/>
       <c r="P102" s="11"/>
     </row>
     <row r="103" spans="3:16">
       <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11" t="s">
-        <v>202</v>
-      </c>
+      <c r="D103" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E103" s="11"/>
       <c r="F103" s="11"/>
       <c r="G103" s="11"/>
-      <c r="H103" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H103" s="11"/>
       <c r="I103" s="11"/>
       <c r="J103" s="11"/>
       <c r="K103" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L103" s="11"/>
+        <v>246</v>
+      </c>
+      <c r="L103" s="11" t="s">
+        <v>272</v>
+      </c>
       <c r="M103" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="N103" s="11"/>
-      <c r="O103" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="N103" s="11" t="s">
         <v>273</v>
       </c>
+      <c r="O103" s="11"/>
       <c r="P103" s="11"/>
     </row>
     <row r="104" spans="3:16">
-      <c r="C104" s="11"/>
+      <c r="C104" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
       <c r="H104" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I104" s="11"/>
       <c r="J104" s="11"/>
       <c r="K104" s="11" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="L104" s="11"/>
       <c r="M104" s="11" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="N104" s="11"/>
-      <c r="O104" s="11" t="s">
-        <v>273</v>
-      </c>
+      <c r="O104" s="11"/>
       <c r="P104" s="11"/>
     </row>
     <row r="105" spans="3:16">
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11" t="s">
-        <v>274</v>
+        <v>206</v>
       </c>
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
       <c r="H105" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I105" s="11"/>
       <c r="J105" s="11"/>
       <c r="K105" s="11" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="L105" s="11"/>
       <c r="M105" s="11" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="N105" s="11"/>
       <c r="O105" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P105" s="11"/>
     </row>
@@ -4253,12 +4251,12 @@
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11" t="s">
-        <v>277</v>
+        <v>151</v>
       </c>
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
       <c r="H106" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I106" s="11"/>
       <c r="J106" s="11"/>
@@ -4267,11 +4265,11 @@
       </c>
       <c r="L106" s="11"/>
       <c r="M106" s="11" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="N106" s="11"/>
       <c r="O106" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P106" s="11"/>
     </row>
@@ -4279,25 +4277,25 @@
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
       <c r="H107" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I107" s="11"/>
       <c r="J107" s="11"/>
       <c r="K107" s="11" t="s">
-        <v>142</v>
+        <v>277</v>
       </c>
       <c r="L107" s="11"/>
       <c r="M107" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N107" s="11"/>
       <c r="O107" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P107" s="11"/>
     </row>
@@ -4305,14 +4303,12 @@
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F108" s="11"/>
-      <c r="G108" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="G108" s="11"/>
       <c r="H108" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
@@ -4321,11 +4317,11 @@
       </c>
       <c r="L108" s="11"/>
       <c r="M108" s="11" t="s">
-        <v>281</v>
+        <v>184</v>
       </c>
       <c r="N108" s="11"/>
       <c r="O108" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P108" s="11"/>
     </row>
@@ -4333,14 +4329,12 @@
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F109" s="11"/>
-      <c r="G109" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="G109" s="11"/>
       <c r="H109" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I109" s="11"/>
       <c r="J109" s="11"/>
@@ -4349,11 +4343,11 @@
       </c>
       <c r="L109" s="11"/>
       <c r="M109" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N109" s="11"/>
       <c r="O109" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P109" s="11"/>
     </row>
@@ -4361,36 +4355,42 @@
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
+      <c r="G110" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H110" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I110" s="11"/>
       <c r="J110" s="11"/>
       <c r="K110" s="11" t="s">
-        <v>285</v>
+        <v>142</v>
       </c>
       <c r="L110" s="11"/>
       <c r="M110" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N110" s="11"/>
-      <c r="O110" s="11"/>
+      <c r="O110" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="P110" s="11"/>
     </row>
     <row r="111" spans="3:16">
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
+      <c r="G111" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H111" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I111" s="11"/>
       <c r="J111" s="11"/>
@@ -4399,11 +4399,11 @@
       </c>
       <c r="L111" s="11"/>
       <c r="M111" s="11" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="N111" s="11"/>
       <c r="O111" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P111" s="11"/>
     </row>
@@ -4411,51 +4411,49 @@
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11"/>
       <c r="H112" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I112" s="11"/>
       <c r="J112" s="11"/>
       <c r="K112" s="11" t="s">
-        <v>142</v>
+        <v>287</v>
       </c>
       <c r="L112" s="11"/>
       <c r="M112" s="11" t="s">
-        <v>183</v>
+        <v>288</v>
       </c>
       <c r="N112" s="11"/>
-      <c r="O112" s="11" t="s">
-        <v>273</v>
-      </c>
+      <c r="O112" s="11"/>
       <c r="P112" s="11"/>
     </row>
     <row r="113" spans="3:16">
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11" t="s">
-        <v>11</v>
+        <v>289</v>
       </c>
       <c r="F113" s="11"/>
       <c r="G113" s="11"/>
       <c r="H113" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I113" s="11"/>
       <c r="J113" s="11"/>
       <c r="K113" s="11" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="L113" s="11"/>
       <c r="M113" s="11" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="N113" s="11"/>
       <c r="O113" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P113" s="11"/>
     </row>
@@ -4463,12 +4461,12 @@
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="F114" s="11"/>
       <c r="G114" s="11"/>
       <c r="H114" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I114" s="11"/>
       <c r="J114" s="11"/>
@@ -4477,53 +4475,51 @@
       </c>
       <c r="L114" s="11"/>
       <c r="M114" s="11" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="N114" s="11"/>
       <c r="O114" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P114" s="11"/>
     </row>
     <row r="115" spans="3:16">
       <c r="C115" s="11"/>
-      <c r="D115" s="11" t="s">
-        <v>289</v>
-      </c>
+      <c r="D115" s="11"/>
       <c r="E115" s="11" t="s">
-        <v>290</v>
+        <v>11</v>
       </c>
       <c r="F115" s="11"/>
       <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
+      <c r="H115" s="11" t="s">
+        <v>274</v>
+      </c>
       <c r="I115" s="11"/>
       <c r="J115" s="11"/>
       <c r="K115" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="L115" s="11" t="s">
-        <v>291</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="L115" s="11"/>
       <c r="M115" s="11" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
       <c r="N115" s="11"/>
       <c r="O115" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P115" s="11"/>
     </row>
     <row r="116" spans="3:16">
       <c r="C116" s="11"/>
-      <c r="D116" s="11" t="s">
-        <v>293</v>
-      </c>
+      <c r="D116" s="11"/>
       <c r="E116" s="11" t="s">
-        <v>294</v>
+        <v>146</v>
       </c>
       <c r="F116" s="11"/>
       <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
+      <c r="H116" s="11" t="s">
+        <v>274</v>
+      </c>
       <c r="I116" s="11"/>
       <c r="J116" s="11"/>
       <c r="K116" s="11" t="s">
@@ -4531,49 +4527,49 @@
       </c>
       <c r="L116" s="11"/>
       <c r="M116" s="11" t="s">
-        <v>295</v>
+        <v>201</v>
       </c>
       <c r="N116" s="11"/>
       <c r="O116" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P116" s="11"/>
     </row>
     <row r="117" spans="3:16">
       <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
+      <c r="D117" s="11" t="s">
+        <v>291</v>
+      </c>
       <c r="E117" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F117" s="11"/>
       <c r="G117" s="11"/>
-      <c r="H117" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H117" s="11"/>
       <c r="I117" s="11"/>
       <c r="J117" s="11"/>
       <c r="K117" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="L117" s="11" t="s">
-        <v>191</v>
+        <v>293</v>
       </c>
       <c r="M117" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N117" s="11"/>
       <c r="O117" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P117" s="11"/>
     </row>
     <row r="118" spans="3:16">
       <c r="C118" s="11"/>
       <c r="D118" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F118" s="11"/>
       <c r="G118" s="11"/>
@@ -4585,49 +4581,49 @@
       </c>
       <c r="L118" s="11"/>
       <c r="M118" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="N118" s="11"/>
       <c r="O118" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P118" s="11"/>
     </row>
     <row r="119" spans="3:16">
       <c r="C119" s="11"/>
-      <c r="D119" s="11" t="s">
-        <v>301</v>
-      </c>
+      <c r="D119" s="11"/>
       <c r="E119" s="11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F119" s="11"/>
       <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
+      <c r="H119" s="11" t="s">
+        <v>274</v>
+      </c>
       <c r="I119" s="11"/>
       <c r="J119" s="11"/>
       <c r="K119" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="L119" s="11"/>
+      <c r="L119" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="M119" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N119" s="11"/>
       <c r="O119" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P119" s="11"/>
     </row>
     <row r="120" spans="3:16">
-      <c r="C120" s="11" t="s">
-        <v>112</v>
-      </c>
+      <c r="C120" s="11"/>
       <c r="D120" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F120" s="11"/>
       <c r="G120" s="11"/>
@@ -4635,25 +4631,25 @@
       <c r="I120" s="11"/>
       <c r="J120" s="11"/>
       <c r="K120" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="L120" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="M120" s="11"/>
+        <v>142</v>
+      </c>
+      <c r="L120" s="11"/>
+      <c r="M120" s="11" t="s">
+        <v>302</v>
+      </c>
       <c r="N120" s="11"/>
-      <c r="O120" s="11"/>
+      <c r="O120" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="P120" s="11"/>
     </row>
     <row r="121" spans="3:16">
-      <c r="C121" s="11" t="s">
-        <v>113</v>
-      </c>
+      <c r="C121" s="11"/>
       <c r="D121" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F121" s="11"/>
       <c r="G121" s="11"/>
@@ -4661,23 +4657,27 @@
       <c r="I121" s="11"/>
       <c r="J121" s="11"/>
       <c r="K121" s="11" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="L121" s="11"/>
       <c r="M121" s="11" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="N121" s="11"/>
-      <c r="O121" s="11"/>
+      <c r="O121" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="P121" s="11"/>
     </row>
     <row r="122" spans="3:16">
-      <c r="C122" s="11"/>
+      <c r="C122" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="D122" s="11" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F122" s="11"/>
       <c r="G122" s="11"/>
@@ -4685,23 +4685,25 @@
       <c r="I122" s="11"/>
       <c r="J122" s="11"/>
       <c r="K122" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="L122" s="11"/>
-      <c r="M122" s="11" t="s">
-        <v>312</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="L122" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="M122" s="11"/>
       <c r="N122" s="11"/>
       <c r="O122" s="11"/>
       <c r="P122" s="11"/>
     </row>
     <row r="123" spans="3:16">
-      <c r="C123" s="11"/>
+      <c r="C123" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D123" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="F123" s="11"/>
       <c r="G123" s="11"/>
@@ -4709,11 +4711,11 @@
       <c r="I123" s="11"/>
       <c r="J123" s="11"/>
       <c r="K123" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L123" s="11"/>
       <c r="M123" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="N123" s="11"/>
       <c r="O123" s="11"/>
@@ -4722,10 +4724,10 @@
     <row r="124" spans="3:16">
       <c r="C124" s="11"/>
       <c r="D124" s="11" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>264</v>
+        <v>313</v>
       </c>
       <c r="F124" s="11"/>
       <c r="G124" s="11"/>
@@ -4733,11 +4735,11 @@
       <c r="I124" s="11"/>
       <c r="J124" s="11"/>
       <c r="K124" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L124" s="11"/>
       <c r="M124" s="11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N124" s="11"/>
       <c r="O124" s="11"/>
@@ -4746,10 +4748,10 @@
     <row r="125" spans="3:16">
       <c r="C125" s="11"/>
       <c r="D125" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="F125" s="11"/>
       <c r="G125" s="11"/>
@@ -4757,11 +4759,11 @@
       <c r="I125" s="11"/>
       <c r="J125" s="11"/>
       <c r="K125" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L125" s="11"/>
       <c r="M125" s="11" t="s">
-        <v>230</v>
+        <v>316</v>
       </c>
       <c r="N125" s="11"/>
       <c r="O125" s="11"/>
@@ -4770,10 +4772,10 @@
     <row r="126" spans="3:16">
       <c r="C126" s="11"/>
       <c r="D126" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>320</v>
+        <v>266</v>
       </c>
       <c r="F126" s="11"/>
       <c r="G126" s="11"/>
@@ -4781,11 +4783,11 @@
       <c r="I126" s="11"/>
       <c r="J126" s="11"/>
       <c r="K126" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L126" s="11"/>
       <c r="M126" s="11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N126" s="11"/>
       <c r="O126" s="11"/>
@@ -4794,10 +4796,10 @@
     <row r="127" spans="3:16">
       <c r="C127" s="11"/>
       <c r="D127" s="11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E127" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F127" s="11"/>
       <c r="G127" s="11"/>
@@ -4805,11 +4807,11 @@
       <c r="I127" s="11"/>
       <c r="J127" s="11"/>
       <c r="K127" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L127" s="11"/>
       <c r="M127" s="11" t="s">
-        <v>324</v>
+        <v>233</v>
       </c>
       <c r="N127" s="11"/>
       <c r="O127" s="11"/>
@@ -4818,10 +4820,10 @@
     <row r="128" spans="3:16">
       <c r="C128" s="11"/>
       <c r="D128" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F128" s="11"/>
       <c r="G128" s="11"/>
@@ -4829,39 +4831,35 @@
       <c r="I128" s="11"/>
       <c r="J128" s="11"/>
       <c r="K128" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L128" s="11"/>
       <c r="M128" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="N128" s="11"/>
       <c r="O128" s="11"/>
       <c r="P128" s="11"/>
     </row>
     <row r="129" spans="3:16">
-      <c r="C129" s="11" t="s">
-        <v>115</v>
-      </c>
+      <c r="C129" s="11"/>
       <c r="D129" s="11" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F129" s="11"/>
       <c r="G129" s="11"/>
-      <c r="H129" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H129" s="11"/>
       <c r="I129" s="11"/>
       <c r="J129" s="11"/>
       <c r="K129" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L129" s="11"/>
       <c r="M129" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="N129" s="11"/>
       <c r="O129" s="11"/>
@@ -4870,50 +4868,50 @@
     <row r="130" spans="3:16">
       <c r="C130" s="11"/>
       <c r="D130" s="11" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F130" s="11"/>
       <c r="G130" s="11"/>
-      <c r="H130" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H130" s="11"/>
       <c r="I130" s="11"/>
       <c r="J130" s="11"/>
       <c r="K130" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L130" s="11"/>
       <c r="M130" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="N130" s="11"/>
       <c r="O130" s="11"/>
       <c r="P130" s="11"/>
     </row>
     <row r="131" spans="3:16">
-      <c r="C131" s="11"/>
+      <c r="C131" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="D131" s="11" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="F131" s="11"/>
       <c r="G131" s="11"/>
       <c r="H131" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I131" s="11"/>
       <c r="J131" s="11"/>
       <c r="K131" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L131" s="11"/>
       <c r="M131" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N131" s="11"/>
       <c r="O131" s="11"/>
@@ -4922,54 +4920,50 @@
     <row r="132" spans="3:16">
       <c r="C132" s="11"/>
       <c r="D132" s="11" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F132" s="11"/>
       <c r="G132" s="11"/>
       <c r="H132" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I132" s="11"/>
       <c r="J132" s="11"/>
       <c r="K132" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L132" s="11"/>
       <c r="M132" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="N132" s="11"/>
       <c r="O132" s="11"/>
       <c r="P132" s="11"/>
     </row>
     <row r="133" spans="3:16">
-      <c r="C133" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="C133" s="11"/>
       <c r="D133" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="F133" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F133" s="11"/>
       <c r="G133" s="11"/>
       <c r="H133" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I133" s="11"/>
       <c r="J133" s="11"/>
       <c r="K133" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L133" s="11"/>
       <c r="M133" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N133" s="11"/>
       <c r="O133" s="11"/>
@@ -4978,52 +4972,54 @@
     <row r="134" spans="3:16">
       <c r="C134" s="11"/>
       <c r="D134" s="11" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="F134" s="11"/>
       <c r="G134" s="11"/>
       <c r="H134" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I134" s="11"/>
       <c r="J134" s="11"/>
       <c r="K134" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L134" s="11"/>
       <c r="M134" s="11" t="s">
-        <v>226</v>
+        <v>337</v>
       </c>
       <c r="N134" s="11"/>
       <c r="O134" s="11"/>
       <c r="P134" s="11"/>
     </row>
     <row r="135" spans="3:16">
-      <c r="C135" s="11"/>
+      <c r="C135" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="D135" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>228</v>
+        <v>339</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I135" s="11"/>
       <c r="J135" s="11"/>
       <c r="K135" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L135" s="11"/>
       <c r="M135" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="N135" s="11"/>
       <c r="O135" s="11"/>
@@ -5032,26 +5028,24 @@
     <row r="136" spans="3:16">
       <c r="C136" s="11"/>
       <c r="D136" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="F136" s="11" t="s">
-        <v>345</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F136" s="11"/>
       <c r="G136" s="11"/>
       <c r="H136" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I136" s="11"/>
       <c r="J136" s="11"/>
       <c r="K136" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="L136" s="11"/>
       <c r="M136" s="11" t="s">
-        <v>335</v>
+        <v>229</v>
       </c>
       <c r="N136" s="11"/>
       <c r="O136" s="11"/>
@@ -5060,62 +5054,66 @@
     <row r="137" spans="3:16">
       <c r="C137" s="11"/>
       <c r="D137" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="F137" s="11"/>
+        <v>231</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>343</v>
+      </c>
       <c r="G137" s="11"/>
-      <c r="H137" s="11"/>
+      <c r="H137" s="11" t="s">
+        <v>274</v>
+      </c>
       <c r="I137" s="11"/>
       <c r="J137" s="11"/>
       <c r="K137" s="11" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="L137" s="11"/>
       <c r="M137" s="11" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="N137" s="11"/>
       <c r="O137" s="11"/>
       <c r="P137" s="11"/>
     </row>
     <row r="138" spans="3:16">
-      <c r="C138" s="11" t="s">
-        <v>119</v>
-      </c>
+      <c r="C138" s="11"/>
       <c r="D138" s="11" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="F138" s="11"/>
+        <v>346</v>
+      </c>
+      <c r="F138" s="11" t="s">
+        <v>347</v>
+      </c>
       <c r="G138" s="11"/>
-      <c r="H138" s="11"/>
+      <c r="H138" s="11" t="s">
+        <v>274</v>
+      </c>
       <c r="I138" s="11"/>
       <c r="J138" s="11"/>
       <c r="K138" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="L138" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="M138" s="11"/>
-      <c r="N138" s="11" t="s">
-        <v>353</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L138" s="11"/>
+      <c r="M138" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="N138" s="11"/>
       <c r="O138" s="11"/>
       <c r="P138" s="11"/>
     </row>
     <row r="139" spans="3:16">
       <c r="C139" s="11"/>
       <c r="D139" s="11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="F139" s="11"/>
       <c r="G139" s="11"/>
@@ -5123,25 +5121,25 @@
       <c r="I139" s="11"/>
       <c r="J139" s="11"/>
       <c r="K139" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="L139" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="M139" s="11"/>
-      <c r="N139" s="11" t="s">
-        <v>357</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="L139" s="11"/>
+      <c r="M139" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="N139" s="11"/>
       <c r="O139" s="11"/>
       <c r="P139" s="11"/>
     </row>
     <row r="140" spans="3:16">
-      <c r="C140" s="11"/>
+      <c r="C140" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="D140" s="11" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="F140" s="11"/>
       <c r="G140" s="11"/>
@@ -5149,14 +5147,14 @@
       <c r="I140" s="11"/>
       <c r="J140" s="11"/>
       <c r="K140" s="11" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="L140" s="11" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="M140" s="11"/>
       <c r="N140" s="11" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="O140" s="11"/>
       <c r="P140" s="11"/>
@@ -5164,10 +5162,10 @@
     <row r="141" spans="3:16">
       <c r="C141" s="11"/>
       <c r="D141" s="11" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E141" s="11" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F141" s="11"/>
       <c r="G141" s="11"/>
@@ -5175,27 +5173,25 @@
       <c r="I141" s="11"/>
       <c r="J141" s="11"/>
       <c r="K141" s="11" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="L141" s="11" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="M141" s="11"/>
       <c r="N141" s="11" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="O141" s="11"/>
       <c r="P141" s="11"/>
     </row>
     <row r="142" spans="3:16">
-      <c r="C142" s="11" t="s">
-        <v>121</v>
-      </c>
+      <c r="C142" s="11"/>
       <c r="D142" s="11" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E142" s="11" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="F142" s="11"/>
       <c r="G142" s="11"/>
@@ -5203,14 +5199,14 @@
       <c r="I142" s="11"/>
       <c r="J142" s="11"/>
       <c r="K142" s="11" t="s">
-        <v>244</v>
+        <v>353</v>
       </c>
       <c r="L142" s="11" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="M142" s="11"/>
       <c r="N142" s="11" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
@@ -5218,10 +5214,10 @@
     <row r="143" spans="3:16">
       <c r="C143" s="11"/>
       <c r="D143" s="11" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E143" s="11" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="F143" s="11"/>
       <c r="G143" s="11"/>
@@ -5229,25 +5225,27 @@
       <c r="I143" s="11"/>
       <c r="J143" s="11"/>
       <c r="K143" s="11" t="s">
-        <v>244</v>
+        <v>353</v>
       </c>
       <c r="L143" s="11" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="M143" s="11"/>
       <c r="N143" s="11" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="O143" s="11"/>
       <c r="P143" s="11"/>
     </row>
     <row r="144" spans="3:16">
-      <c r="C144" s="11"/>
+      <c r="C144" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="D144" s="11" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E144" s="11" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F144" s="11"/>
       <c r="G144" s="11"/>
@@ -5255,25 +5253,25 @@
       <c r="I144" s="11"/>
       <c r="J144" s="11"/>
       <c r="K144" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L144" s="11" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="M144" s="11"/>
       <c r="N144" s="11" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="O144" s="11"/>
       <c r="P144" s="11"/>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="3:16">
       <c r="C145" s="11"/>
       <c r="D145" s="11" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="F145" s="11"/>
       <c r="G145" s="11"/>
@@ -5281,25 +5279,25 @@
       <c r="I145" s="11"/>
       <c r="J145" s="11"/>
       <c r="K145" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L145" s="11" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="M145" s="11"/>
       <c r="N145" s="11" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="O145" s="11"/>
       <c r="P145" s="11"/>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="3:16">
       <c r="C146" s="11"/>
       <c r="D146" s="11" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E146" s="11" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="F146" s="11"/>
       <c r="G146" s="11"/>
@@ -5307,25 +5305,25 @@
       <c r="I146" s="11"/>
       <c r="J146" s="11"/>
       <c r="K146" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L146" s="11" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="M146" s="11"/>
       <c r="N146" s="11" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="O146" s="11"/>
       <c r="P146" s="11"/>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="3:16">
       <c r="C147" s="11"/>
       <c r="D147" s="11" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E147" s="11" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="F147" s="11"/>
       <c r="G147" s="11"/>
@@ -5333,25 +5331,25 @@
       <c r="I147" s="11"/>
       <c r="J147" s="11"/>
       <c r="K147" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L147" s="11" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="M147" s="11"/>
       <c r="N147" s="11" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="O147" s="11"/>
       <c r="P147" s="11"/>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="3:16">
       <c r="C148" s="11"/>
       <c r="D148" s="11" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E148" s="11" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="F148" s="11"/>
       <c r="G148" s="11"/>
@@ -5359,25 +5357,25 @@
       <c r="I148" s="11"/>
       <c r="J148" s="11"/>
       <c r="K148" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L148" s="11" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
       <c r="M148" s="11"/>
       <c r="N148" s="11" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="O148" s="11"/>
       <c r="P148" s="11"/>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="3:16">
       <c r="C149" s="11"/>
       <c r="D149" s="11" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E149" s="11" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F149" s="11"/>
       <c r="G149" s="11"/>
@@ -5385,25 +5383,25 @@
       <c r="I149" s="11"/>
       <c r="J149" s="11"/>
       <c r="K149" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L149" s="11" t="s">
-        <v>249</v>
+        <v>390</v>
       </c>
       <c r="M149" s="11"/>
       <c r="N149" s="11" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="O149" s="11"/>
       <c r="P149" s="11"/>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="3:16">
       <c r="C150" s="11"/>
       <c r="D150" s="11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E150" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F150" s="11"/>
       <c r="G150" s="11"/>
@@ -5411,25 +5409,25 @@
       <c r="I150" s="11"/>
       <c r="J150" s="11"/>
       <c r="K150" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L150" s="11" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="M150" s="11"/>
       <c r="N150" s="11" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="O150" s="11"/>
       <c r="P150" s="11"/>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="3:16">
       <c r="C151" s="11"/>
       <c r="D151" s="11" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E151" s="11" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F151" s="11"/>
       <c r="G151" s="11"/>
@@ -5437,286 +5435,312 @@
       <c r="I151" s="11"/>
       <c r="J151" s="11"/>
       <c r="K151" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L151" s="11" t="s">
-        <v>402</v>
+        <v>251</v>
       </c>
       <c r="M151" s="11"/>
       <c r="N151" s="11" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="O151" s="11"/>
       <c r="P151" s="11"/>
     </row>
-    <row r="152" spans="1:16">
-      <c r="C152" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D152" s="11"/>
+    <row r="152" spans="3:16">
+      <c r="C152" s="11"/>
+      <c r="D152" s="11" t="s">
+        <v>398</v>
+      </c>
       <c r="E152" s="11" t="s">
-        <v>190</v>
+        <v>399</v>
       </c>
       <c r="F152" s="11"/>
       <c r="G152" s="11"/>
-      <c r="H152" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H152" s="11"/>
       <c r="I152" s="11"/>
       <c r="J152" s="11"/>
-      <c r="K152" s="11"/>
-      <c r="L152" s="11"/>
-      <c r="M152" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="N152" s="11"/>
+      <c r="K152" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L152" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="M152" s="11"/>
+      <c r="N152" s="11" t="s">
+        <v>401</v>
+      </c>
       <c r="O152" s="11"/>
       <c r="P152" s="11"/>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="3:16">
       <c r="C153" s="11"/>
-      <c r="D153" s="11"/>
+      <c r="D153" s="11" t="s">
+        <v>402</v>
+      </c>
       <c r="E153" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F153" s="11"/>
       <c r="G153" s="11"/>
-      <c r="H153" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="H153" s="11"/>
       <c r="I153" s="11"/>
       <c r="J153" s="11"/>
-      <c r="K153" s="11"/>
-      <c r="L153" s="11"/>
-      <c r="M153" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="N153" s="11"/>
+      <c r="K153" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L153" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="M153" s="11"/>
+      <c r="N153" s="11" t="s">
+        <v>405</v>
+      </c>
       <c r="O153" s="11"/>
       <c r="P153" s="11"/>
     </row>
-    <row r="154" spans="1:16">
-      <c r="C154" s="11"/>
+    <row r="154" spans="3:16">
+      <c r="C154" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F154" s="11"/>
       <c r="G154" s="11"/>
       <c r="H154" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I154" s="11"/>
       <c r="J154" s="11"/>
       <c r="K154" s="11"/>
       <c r="L154" s="11"/>
       <c r="M154" s="11" t="s">
-        <v>197</v>
+        <v>406</v>
       </c>
       <c r="N154" s="11"/>
       <c r="O154" s="11"/>
       <c r="P154" s="11"/>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="3:16">
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11" t="s">
-        <v>11</v>
+        <v>407</v>
       </c>
       <c r="F155" s="11"/>
       <c r="G155" s="11"/>
       <c r="H155" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I155" s="11"/>
       <c r="J155" s="11"/>
       <c r="K155" s="11"/>
       <c r="L155" s="11"/>
       <c r="M155" s="11" t="s">
-        <v>185</v>
+        <v>408</v>
       </c>
       <c r="N155" s="11"/>
       <c r="O155" s="11"/>
       <c r="P155" s="11"/>
     </row>
-    <row r="156" spans="1:16">
-      <c r="C156" s="5" t="s">
+    <row r="156" spans="3:16">
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F156" s="11"/>
+      <c r="G156" s="11"/>
+      <c r="H156" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="I156" s="11"/>
+      <c r="J156" s="11"/>
+      <c r="K156" s="11"/>
+      <c r="L156" s="11"/>
+      <c r="M156" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="N156" s="11"/>
+      <c r="O156" s="11"/>
+      <c r="P156" s="11"/>
+    </row>
+    <row r="157" spans="3:16">
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
+      <c r="E157" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="11"/>
+      <c r="G157" s="11"/>
+      <c r="H157" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="I157" s="11"/>
+      <c r="J157" s="11"/>
+      <c r="K157" s="11"/>
+      <c r="L157" s="11"/>
+      <c r="M157" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="N157" s="11"/>
+      <c r="O157" s="11"/>
+      <c r="P157" s="11"/>
+    </row>
+    <row r="158" spans="3:16">
+      <c r="C158" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="3"/>
-      <c r="H156" s="3"/>
-      <c r="I156" s="3"/>
-      <c r="J156" s="3"/>
-      <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
-      <c r="M156" s="3"/>
-      <c r="N156" s="3"/>
-      <c r="O156" s="3"/>
-      <c r="P156" s="3"/>
-    </row>
-    <row r="160" spans="1:16">
-      <c r="A160" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C160" s="3" t="s">
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="3"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="3"/>
+      <c r="K158" s="3"/>
+      <c r="L158" s="3"/>
+      <c r="M158" s="3"/>
+      <c r="N158" s="3"/>
+      <c r="O158" s="3"/>
+      <c r="P158" s="3"/>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="B162" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="D162" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E162" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
-    </row>
-    <row r="162" spans="1:11">
-      <c r="C162" s="5" t="s">
+    <row r="163" spans="1:11">
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="11"/>
+    </row>
+    <row r="164" spans="1:11">
+      <c r="C164" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-    </row>
-    <row r="165" spans="1:11">
-      <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="1:11">
-      <c r="A166" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C166" s="3" t="s">
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+    </row>
+    <row r="167" spans="1:11">
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="1:11">
+      <c r="A168" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D166" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="F166" s="3" t="s">
+      <c r="D168" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="G166" s="3" t="s">
+      <c r="E168" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="G168" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
-      <c r="C167" s="11"/>
-      <c r="D167" s="11"/>
-      <c r="E167" s="11"/>
-      <c r="F167" s="11"/>
-      <c r="G167" s="11"/>
-    </row>
-    <row r="168" spans="1:11">
-      <c r="C168" s="5" t="s">
+    <row r="169" spans="1:11">
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="11"/>
+    </row>
+    <row r="170" spans="1:11">
+      <c r="C170" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D168" s="3"/>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-    </row>
-    <row r="171" spans="1:11">
-      <c r="B171" s="16" t="s">
-        <v>415</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11">
-      <c r="A172" s="12" t="s">
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="B173" s="16" t="s">
         <v>417</v>
       </c>
-      <c r="B172" s="13"/>
-      <c r="C172" s="17" t="s">
+      <c r="E173" s="8" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
+      <c r="A174" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B174" s="13"/>
+      <c r="C174" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D172" s="17" t="s">
+      <c r="D174" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="E172" s="17" t="s">
-        <v>418</v>
-      </c>
-      <c r="F172" s="17" t="s">
-        <v>419</v>
-      </c>
-      <c r="G172" s="17" t="s">
+      <c r="E174" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="H172" s="17" t="s">
+      <c r="F174" s="17" t="s">
         <v>421</v>
       </c>
-      <c r="I172" s="17" t="s">
+      <c r="G174" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="H174" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="I174" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K172" s="8" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11">
-      <c r="C173" s="11" t="s">
+      <c r="K174" s="8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="C175" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D173" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="E173" s="11" t="s">
+      <c r="D175" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E175" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="F173" s="11"/>
-      <c r="G173" s="11"/>
-      <c r="H173" s="11"/>
-      <c r="I173" s="11"/>
-      <c r="K173" s="8" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11">
-      <c r="C174" s="11"/>
-      <c r="D174" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="E174" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F174" s="11"/>
-      <c r="G174" s="11"/>
-      <c r="H174" s="11"/>
-      <c r="I174" s="11"/>
-    </row>
-    <row r="175" spans="1:11">
-      <c r="C175" s="11"/>
-      <c r="D175" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E175" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="F175" s="11"/>
       <c r="G175" s="11"/>
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
+      <c r="K175" s="8" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="176" spans="1:11">
       <c r="C176" s="11"/>
       <c r="D176" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E176" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F176" s="11"/>
       <c r="G176" s="11"/>
@@ -5726,10 +5750,10 @@
     <row r="177" spans="3:9">
       <c r="C177" s="11"/>
       <c r="D177" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E177" s="11" t="s">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="F177" s="11"/>
       <c r="G177" s="11"/>
@@ -5739,14 +5763,12 @@
     <row r="178" spans="3:9">
       <c r="C178" s="11"/>
       <c r="D178" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E178" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E178" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="F178" s="11" t="s">
-        <v>187</v>
-      </c>
+      <c r="F178" s="11"/>
       <c r="G178" s="11"/>
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
@@ -5754,12 +5776,12 @@
     <row r="179" spans="3:9">
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E179" s="11"/>
-      <c r="F179" s="11" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="E179" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F179" s="11"/>
       <c r="G179" s="11"/>
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
@@ -5767,12 +5789,14 @@
     <row r="180" spans="3:9">
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E180" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="F180" s="11"/>
+        <v>144</v>
+      </c>
+      <c r="F180" s="11" t="s">
+        <v>191</v>
+      </c>
       <c r="G180" s="11"/>
       <c r="H180" s="11"/>
       <c r="I180" s="11"/>
@@ -5780,13 +5804,11 @@
     <row r="181" spans="3:9">
       <c r="C181" s="11"/>
       <c r="D181" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E181" s="11" t="s">
-        <v>424</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="E181" s="11"/>
       <c r="F181" s="11" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="G181" s="11"/>
       <c r="H181" s="11"/>
@@ -5795,12 +5817,12 @@
     <row r="182" spans="3:9">
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E182" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E182" s="11"/>
-      <c r="F182" s="11" t="s">
-        <v>199</v>
-      </c>
+      <c r="F182" s="11"/>
       <c r="G182" s="11"/>
       <c r="H182" s="11"/>
       <c r="I182" s="11"/>
@@ -5808,13 +5830,13 @@
     <row r="183" spans="3:9">
       <c r="C183" s="11"/>
       <c r="D183" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E183" s="11" t="s">
-        <v>151</v>
+        <v>426</v>
       </c>
       <c r="F183" s="11" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="G183" s="11"/>
       <c r="H183" s="11"/>
@@ -5823,11 +5845,11 @@
     <row r="184" spans="3:9">
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E184" s="11"/>
       <c r="F184" s="11" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="G184" s="11"/>
       <c r="H184" s="11"/>
@@ -5836,27 +5858,27 @@
     <row r="185" spans="3:9">
       <c r="C185" s="11"/>
       <c r="D185" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E185" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F185" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E185" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="F185" s="11"/>
       <c r="G185" s="11"/>
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
     </row>
     <row r="186" spans="3:9">
-      <c r="C186" s="11" t="s">
-        <v>113</v>
-      </c>
+      <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="E186" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="F186" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="E186" s="11"/>
+      <c r="F186" s="11" t="s">
+        <v>191</v>
+      </c>
       <c r="G186" s="11"/>
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
@@ -5864,10 +5886,10 @@
     <row r="187" spans="3:9">
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
-        <v>310</v>
+        <v>210</v>
       </c>
       <c r="E187" s="11" t="s">
-        <v>311</v>
+        <v>427</v>
       </c>
       <c r="F187" s="11"/>
       <c r="G187" s="11"/>
@@ -5875,12 +5897,14 @@
       <c r="I187" s="11"/>
     </row>
     <row r="188" spans="3:9">
-      <c r="C188" s="11"/>
+      <c r="C188" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D188" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E188" s="11" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="F188" s="11"/>
       <c r="G188" s="11"/>
@@ -5890,224 +5914,250 @@
     <row r="189" spans="3:9">
       <c r="C189" s="11"/>
       <c r="D189" s="11" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E189" s="11" t="s">
-        <v>264</v>
+        <v>313</v>
       </c>
       <c r="F189" s="11"/>
       <c r="G189" s="11"/>
-      <c r="H189" s="11" t="s">
-        <v>426</v>
-      </c>
+      <c r="H189" s="11"/>
       <c r="I189" s="11"/>
     </row>
     <row r="190" spans="3:9">
       <c r="C190" s="11"/>
       <c r="D190" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E190" s="11" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="F190" s="11"/>
       <c r="G190" s="11"/>
-      <c r="H190" s="11" t="s">
-        <v>427</v>
-      </c>
+      <c r="H190" s="11"/>
       <c r="I190" s="11"/>
     </row>
     <row r="191" spans="3:9">
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E191" s="11" t="s">
-        <v>320</v>
+        <v>266</v>
       </c>
       <c r="F191" s="11"/>
       <c r="G191" s="11"/>
       <c r="H191" s="11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I191" s="11"/>
     </row>
     <row r="192" spans="3:9">
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E192" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F192" s="11"/>
       <c r="G192" s="11"/>
       <c r="H192" s="11" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I192" s="11"/>
     </row>
     <row r="193" spans="3:9">
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E193" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F193" s="11"/>
       <c r="G193" s="11"/>
       <c r="H193" s="11" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I193" s="11"/>
     </row>
     <row r="194" spans="3:9">
-      <c r="C194" s="11" t="s">
-        <v>115</v>
-      </c>
+      <c r="C194" s="11"/>
       <c r="D194" s="11" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F194" s="11"/>
       <c r="G194" s="11"/>
-      <c r="H194" s="11"/>
+      <c r="H194" s="11" t="s">
+        <v>429</v>
+      </c>
       <c r="I194" s="11"/>
     </row>
     <row r="195" spans="3:9">
       <c r="C195" s="11"/>
       <c r="D195" s="11" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="E195" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F195" s="11"/>
       <c r="G195" s="11"/>
-      <c r="H195" s="11"/>
+      <c r="H195" s="11" t="s">
+        <v>429</v>
+      </c>
       <c r="I195" s="11"/>
     </row>
     <row r="196" spans="3:9">
-      <c r="C196" s="11"/>
+      <c r="C196" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="D196" s="11" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="E196" s="11" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
       <c r="F196" s="11"/>
       <c r="G196" s="11"/>
-      <c r="H196" s="11" t="s">
-        <v>428</v>
-      </c>
+      <c r="H196" s="11"/>
       <c r="I196" s="11"/>
     </row>
     <row r="197" spans="3:9">
       <c r="C197" s="11"/>
       <c r="D197" s="11" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="E197" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F197" s="11"/>
       <c r="G197" s="11"/>
-      <c r="H197" s="11" t="s">
-        <v>427</v>
-      </c>
+      <c r="H197" s="11"/>
       <c r="I197" s="11"/>
     </row>
     <row r="198" spans="3:9">
-      <c r="C198" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="C198" s="11"/>
       <c r="D198" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E198" s="11" t="s">
-        <v>337</v>
+        <v>228</v>
       </c>
       <c r="F198" s="11"/>
       <c r="G198" s="11"/>
-      <c r="H198" s="11"/>
+      <c r="H198" s="11" t="s">
+        <v>430</v>
+      </c>
       <c r="I198" s="11"/>
     </row>
     <row r="199" spans="3:9">
       <c r="C199" s="11"/>
       <c r="D199" s="11" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="E199" s="11" t="s">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="F199" s="11"/>
       <c r="G199" s="11"/>
       <c r="H199" s="11" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="I199" s="11"/>
     </row>
     <row r="200" spans="3:9">
-      <c r="C200" s="11"/>
+      <c r="C200" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="D200" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E200" s="11" t="s">
-        <v>228</v>
+        <v>339</v>
       </c>
       <c r="F200" s="11"/>
       <c r="G200" s="11"/>
-      <c r="H200" s="11" t="s">
-        <v>427</v>
-      </c>
+      <c r="H200" s="11"/>
       <c r="I200" s="11"/>
     </row>
     <row r="201" spans="3:9">
       <c r="C201" s="11"/>
       <c r="D201" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E201" s="11" t="s">
-        <v>344</v>
+        <v>228</v>
       </c>
       <c r="F201" s="11"/>
       <c r="G201" s="11"/>
       <c r="H201" s="11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I201" s="11"/>
     </row>
     <row r="202" spans="3:9">
       <c r="C202" s="11"/>
       <c r="D202" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E202" s="11" t="s">
-        <v>347</v>
+        <v>231</v>
       </c>
       <c r="F202" s="11"/>
       <c r="G202" s="11"/>
       <c r="H202" s="11" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I202" s="11"/>
     </row>
     <row r="203" spans="3:9">
-      <c r="C203" s="5" t="s">
+      <c r="C203" s="11"/>
+      <c r="D203" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="E203" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="F203" s="11"/>
+      <c r="G203" s="11"/>
+      <c r="H203" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="I203" s="11"/>
+    </row>
+    <row r="204" spans="3:9">
+      <c r="C204" s="11"/>
+      <c r="D204" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E204" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F204" s="11"/>
+      <c r="G204" s="11"/>
+      <c r="H204" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="I204" s="11"/>
+    </row>
+    <row r="205" spans="3:9">
+      <c r="C205" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D203" s="3"/>
-      <c r="E203" s="3"/>
-      <c r="F203" s="3"/>
-      <c r="G203" s="3"/>
-      <c r="H203" s="3"/>
-      <c r="I203" s="3"/>
-    </row>
-    <row r="204" spans="3:9">
-      <c r="H204" s="8"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="3"/>
+      <c r="I205" s="3"/>
+    </row>
+    <row r="206" spans="3:9">
+      <c r="H206" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6148,7 +6198,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
Bugfix: fix apps/es: ES005 settle button error
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES005.xlsx
+++ b/apps/es/resources/screen/ES005.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all-workspace\python\VsCodeProjects\wci2\es\resources\screen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53B1B1-4ADB-4C96-BB69-84D5FCB434C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1005" yWindow="-105" windowWidth="29040" windowHeight="4170"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="View Dfn" sheetId="1" r:id="rId1"/>
     <sheet name="Widgets" sheetId="2" r:id="rId2"/>
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1195,112 +1201,112 @@
     <t>Settle</t>
   </si>
   <si>
-    <t>settle(hdrFg, uploadFg)</t>
-  </si>
-  <si>
-    <t>bttRevertSettledPayment</t>
-  </si>
-  <si>
-    <t>Revert Settled Payment</t>
-  </si>
-  <si>
-    <t>icon:images/cancel_button.gif
-dialog:content: Are you sure to revert this settled payment?</t>
-  </si>
-  <si>
-    <t>revertSettledPayment(hdrFg)</t>
-  </si>
-  <si>
-    <t>operate_dt</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>operator.usr_nm</t>
-  </si>
-  <si>
-    <t>subScreenTable</t>
-  </si>
-  <si>
-    <t>Sub Screen</t>
-  </si>
-  <si>
-    <t>Sub Screen Name</t>
-  </si>
-  <si>
-    <t>fieldGroupLinkTable</t>
-  </si>
-  <si>
-    <t>Field Group Links</t>
-  </si>
-  <si>
-    <t>Local Key</t>
-  </si>
-  <si>
-    <t>Parent Field Group Name</t>
-  </si>
-  <si>
-    <t>Parent Key</t>
-  </si>
-  <si>
-    <t>Table Header and Footer for Field Groups</t>
-  </si>
-  <si>
-    <t>add as many levels as needed</t>
-  </si>
-  <si>
-    <t>headerFooterTable</t>
-  </si>
-  <si>
-    <t>Header Level 1</t>
-  </si>
-  <si>
-    <t>Header Level 2</t>
-  </si>
-  <si>
-    <t>Header Level 3</t>
-  </si>
-  <si>
-    <t>Footer</t>
-  </si>
-  <si>
-    <t>optional for table field groups only</t>
-  </si>
-  <si>
-    <t>this is only an example, does not match the above definition</t>
-  </si>
-  <si>
-    <t>Expense Status</t>
-  </si>
-  <si>
-    <t>PO NO.</t>
-  </si>
-  <si>
-    <t>text: "Sum:"</t>
-  </si>
-  <si>
-    <t>formula:"sum"</t>
-  </si>
-  <si>
-    <t>text: "Sum"</t>
-  </si>
-  <si>
-    <t>One tailor made javascript for each layout</t>
-  </si>
-  <si>
-    <t>202505261706</t>
-  </si>
-  <si>
     <t>icon: images/action_button.gif
 type: uploadButton
 dialog: title:Confirm settle;continueName:Yes;content:Are you sure to settle this expense?</t>
+  </si>
+  <si>
+    <t>settle(hdrFg, uploadFg)</t>
+  </si>
+  <si>
+    <t>bttRevertSettledPayment</t>
+  </si>
+  <si>
+    <t>Revert Settled Payment</t>
+  </si>
+  <si>
+    <t>icon:images/cancel_button.gif
+dialog:content: Are you sure to revert this settled payment?</t>
+  </si>
+  <si>
+    <t>revertSettledPayment(hdrFg)</t>
+  </si>
+  <si>
+    <t>operate_dt</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>operator.usr_nm</t>
+  </si>
+  <si>
+    <t>subScreenTable</t>
+  </si>
+  <si>
+    <t>Sub Screen</t>
+  </si>
+  <si>
+    <t>Sub Screen Name</t>
+  </si>
+  <si>
+    <t>fieldGroupLinkTable</t>
+  </si>
+  <si>
+    <t>Field Group Links</t>
+  </si>
+  <si>
+    <t>Local Key</t>
+  </si>
+  <si>
+    <t>Parent Field Group Name</t>
+  </si>
+  <si>
+    <t>Parent Key</t>
+  </si>
+  <si>
+    <t>Table Header and Footer for Field Groups</t>
+  </si>
+  <si>
+    <t>add as many levels as needed</t>
+  </si>
+  <si>
+    <t>headerFooterTable</t>
+  </si>
+  <si>
+    <t>Header Level 1</t>
+  </si>
+  <si>
+    <t>Header Level 2</t>
+  </si>
+  <si>
+    <t>Header Level 3</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>optional for table field groups only</t>
+  </si>
+  <si>
+    <t>this is only an example, does not match the above definition</t>
+  </si>
+  <si>
+    <t>Expense Status</t>
+  </si>
+  <si>
+    <t>PO NO.</t>
+  </si>
+  <si>
+    <t>text: "Sum:"</t>
+  </si>
+  <si>
+    <t>formula:"sum"</t>
+  </si>
+  <si>
+    <t>text: "Sum"</t>
+  </si>
+  <si>
+    <t>One tailor made javascript for each layout</t>
+  </si>
+  <si>
+    <t>20250527115500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1494,15 +1500,15 @@
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 2 2 2" xfId="8"/>
-    <cellStyle name="Normal 2 3" xfId="7"/>
-    <cellStyle name="Normal 2 4" xfId="4"/>
-    <cellStyle name="Normal 2 5" xfId="9"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Percent 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1510,8 +1516,65 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1314450" y="1314450"/>
+          <a:ext cx="4772025" cy="4314825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1589,7 +1652,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1624,7 +1686,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1800,12 +1861,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T195"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L141" sqref="L141"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2063,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>37</v>
@@ -4867,7 +4928,7 @@
       <c r="I133" s="11"/>
       <c r="J133" s="11"/>
       <c r="K133" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L133" s="11" t="s">
         <v>351</v>
@@ -4893,7 +4954,7 @@
       <c r="I134" s="11"/>
       <c r="J134" s="11"/>
       <c r="K134" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L134" s="11" t="s">
         <v>355</v>
@@ -4919,7 +4980,7 @@
       <c r="I135" s="11"/>
       <c r="J135" s="11"/>
       <c r="K135" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L135" s="11" t="s">
         <v>359</v>
@@ -4945,7 +5006,7 @@
       <c r="I136" s="11"/>
       <c r="J136" s="11"/>
       <c r="K136" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L136" s="11" t="s">
         <v>363</v>
@@ -4971,7 +5032,7 @@
       <c r="I137" s="11"/>
       <c r="J137" s="11"/>
       <c r="K137" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L137" s="11" t="s">
         <v>367</v>
@@ -4997,7 +5058,7 @@
       <c r="I138" s="11"/>
       <c r="J138" s="11"/>
       <c r="K138" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L138" s="11" t="s">
         <v>371</v>
@@ -5023,7 +5084,7 @@
       <c r="I139" s="11"/>
       <c r="J139" s="11"/>
       <c r="K139" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L139" s="11" t="s">
         <v>339</v>
@@ -5049,7 +5110,7 @@
       <c r="I140" s="11"/>
       <c r="J140" s="11"/>
       <c r="K140" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L140" s="11" t="s">
         <v>255</v>
@@ -5075,14 +5136,14 @@
       <c r="I141" s="11"/>
       <c r="J141" s="11"/>
       <c r="K141" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L141" s="19" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="M141" s="11"/>
       <c r="N141" s="11" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="O141" s="11"/>
       <c r="P141" s="11"/>
@@ -5090,10 +5151,10 @@
     <row r="142" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C142" s="11"/>
       <c r="D142" s="11" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E142" s="11" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F142" s="11"/>
       <c r="G142" s="11"/>
@@ -5101,14 +5162,14 @@
       <c r="I142" s="11"/>
       <c r="J142" s="11"/>
       <c r="K142" s="11" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="L142" s="11" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M142" s="11"/>
       <c r="N142" s="11" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
@@ -5131,7 +5192,7 @@
       <c r="K143" s="11"/>
       <c r="L143" s="11"/>
       <c r="M143" s="11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N143" s="11"/>
       <c r="O143" s="11"/>
@@ -5141,7 +5202,7 @@
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F144" s="11"/>
       <c r="G144" s="11"/>
@@ -5153,7 +5214,7 @@
       <c r="K144" s="11"/>
       <c r="L144" s="11"/>
       <c r="M144" s="11" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N144" s="11"/>
       <c r="O144" s="11"/>
@@ -5223,13 +5284,13 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>77</v>
@@ -5255,22 +5316,22 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>39</v>
@@ -5294,15 +5355,15 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B162" s="16" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B163" s="13"/>
       <c r="C163" s="17" t="s">
@@ -5312,22 +5373,22 @@
         <v>135</v>
       </c>
       <c r="E163" s="17" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I163" s="17" t="s">
         <v>39</v>
       </c>
       <c r="K163" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
@@ -5345,7 +5406,7 @@
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
       <c r="K164" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
@@ -5447,7 +5508,7 @@
         <v>204</v>
       </c>
       <c r="E172" s="11" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F172" s="11" t="s">
         <v>144</v>
@@ -5503,7 +5564,7 @@
         <v>214</v>
       </c>
       <c r="E176" s="11" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F176" s="11"/>
       <c r="G176" s="11"/>
@@ -5562,7 +5623,7 @@
       <c r="F180" s="11"/>
       <c r="G180" s="11"/>
       <c r="H180" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="I180" s="11"/>
     </row>
@@ -5577,7 +5638,7 @@
       <c r="F181" s="11"/>
       <c r="G181" s="11"/>
       <c r="H181" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I181" s="11"/>
     </row>
@@ -5592,7 +5653,7 @@
       <c r="F182" s="11"/>
       <c r="G182" s="11"/>
       <c r="H182" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I182" s="11"/>
     </row>
@@ -5607,7 +5668,7 @@
       <c r="F183" s="11"/>
       <c r="G183" s="11"/>
       <c r="H183" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I183" s="11"/>
     </row>
@@ -5622,7 +5683,7 @@
       <c r="F184" s="11"/>
       <c r="G184" s="11"/>
       <c r="H184" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I184" s="11"/>
     </row>
@@ -5665,7 +5726,7 @@
       <c r="F187" s="11"/>
       <c r="G187" s="11"/>
       <c r="H187" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="I187" s="11"/>
     </row>
@@ -5680,7 +5741,7 @@
       <c r="F188" s="11"/>
       <c r="G188" s="11"/>
       <c r="H188" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I188" s="11"/>
     </row>
@@ -5710,7 +5771,7 @@
       <c r="F190" s="11"/>
       <c r="G190" s="11"/>
       <c r="H190" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="I190" s="11"/>
     </row>
@@ -5725,7 +5786,7 @@
       <c r="F191" s="11"/>
       <c r="G191" s="11"/>
       <c r="H191" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I191" s="11"/>
     </row>
@@ -5740,7 +5801,7 @@
       <c r="F192" s="11"/>
       <c r="G192" s="11"/>
       <c r="H192" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I192" s="11"/>
     </row>
@@ -5755,7 +5816,7 @@
       <c r="F193" s="11"/>
       <c r="G193" s="11"/>
       <c r="H193" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I193" s="11"/>
     </row>
@@ -5781,7 +5842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -5794,7 +5855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A5:C32"/>
   <sheetViews>
@@ -5812,7 +5873,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5827,5 +5888,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bugfix apps/es/resources/screen/ES005.xlsx: Fix number display problem.
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES005.xlsx
+++ b/apps/es/resources/screen/ES005.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all-workspace\python\VsCodeProjects\wci2\es\resources\screen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53B1B1-4ADB-4C96-BB69-84D5FCB434C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1005" yWindow="-105" windowWidth="29040" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="View Dfn" sheetId="1" r:id="rId1"/>
     <sheet name="Widgets" sheetId="2" r:id="rId2"/>
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="414">
   <si>
     <t>Do not modify this column</t>
   </si>
@@ -756,7 +751,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>format: 0.0</t>
+    <t>format: #,###.00</t>
   </si>
   <si>
     <t>amt</t>
@@ -1300,14 +1295,14 @@
     <t>One tailor made javascript for each layout</t>
   </si>
   <si>
-    <t>20250527115500</t>
+    <t>20250529092300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1448,7 +1443,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1494,32 +1489,21 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 2 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="5"/>
+    <cellStyle name="Normal 2 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 3" xfId="7"/>
+    <cellStyle name="Normal 2 4" xfId="4"/>
+    <cellStyle name="Normal 2 5" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1540,13 +1524,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1861,15 +1839,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T195"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1896,7 +1874,7 @@
     <col min="29" max="31" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1905,10 +1883,10 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1919,7 +1897,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1932,7 +1910,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1945,7 +1923,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1960,7 +1938,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1975,7 +1953,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1988,7 +1966,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
@@ -2001,7 +1979,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -2014,7 +1992,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -2027,7 +2005,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -2042,7 +2020,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -2055,7 +2033,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
@@ -2070,7 +2048,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -2081,13 +2059,13 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="6"/>
       <c r="I16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="6"/>
       <c r="C17" s="9" t="s">
         <v>40</v>
@@ -2101,7 +2079,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2130,7 +2108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" s="6"/>
       <c r="C19" s="11" t="s">
         <v>50</v>
@@ -2146,7 +2124,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="C20" s="11" t="s">
         <v>53</v>
       </c>
@@ -2161,7 +2139,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="C21" s="11" t="s">
         <v>55</v>
       </c>
@@ -2176,7 +2154,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="C22" s="11" t="s">
         <v>57</v>
       </c>
@@ -2191,7 +2169,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="C23" s="11" t="s">
         <v>58</v>
       </c>
@@ -2206,7 +2184,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="C24" s="11" t="s">
         <v>60</v>
       </c>
@@ -2221,7 +2199,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="C25" s="11" t="s">
         <v>61</v>
       </c>
@@ -2236,7 +2214,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="C26" s="11" t="s">
         <v>62</v>
       </c>
@@ -2253,7 +2231,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="C27" s="11" t="s">
         <v>66</v>
       </c>
@@ -2268,7 +2246,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" s="6"/>
       <c r="C28" s="5" t="s">
         <v>68</v>
@@ -2280,10 +2258,10 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" s="6"/>
       <c r="D30" s="9" t="s">
         <v>69</v>
@@ -2292,7 +2270,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" s="6"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
@@ -2322,7 +2300,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" s="7" t="s">
         <v>76</v>
       </c>
@@ -2384,7 +2362,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20">
       <c r="B33" s="1"/>
       <c r="C33" s="11" t="s">
         <v>93</v>
@@ -2415,7 +2393,7 @@
       <c r="S33" s="11"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20">
       <c r="C34" s="11" t="s">
         <v>95</v>
       </c>
@@ -2441,7 +2419,7 @@
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20">
       <c r="C35" s="11" t="s">
         <v>98</v>
       </c>
@@ -2475,7 +2453,7 @@
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20">
       <c r="C36" s="11" t="s">
         <v>102</v>
       </c>
@@ -2503,7 +2481,7 @@
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20">
       <c r="C37" s="11" t="s">
         <v>105</v>
       </c>
@@ -2533,7 +2511,7 @@
       <c r="S37" s="11"/>
       <c r="T37" s="11"/>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20">
       <c r="C38" s="11" t="s">
         <v>108</v>
       </c>
@@ -2561,7 +2539,7 @@
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20">
       <c r="C39" s="11" t="s">
         <v>110</v>
       </c>
@@ -2587,7 +2565,7 @@
       <c r="S39" s="11"/>
       <c r="T39" s="11"/>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20">
       <c r="C40" s="11" t="s">
         <v>111</v>
       </c>
@@ -2617,7 +2595,7 @@
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20">
       <c r="C41" s="11" t="s">
         <v>113</v>
       </c>
@@ -2647,7 +2625,7 @@
       <c r="S41" s="11"/>
       <c r="T41" s="11"/>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20">
       <c r="C42" s="11" t="s">
         <v>115</v>
       </c>
@@ -2679,7 +2657,7 @@
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20">
       <c r="C43" s="11" t="s">
         <v>117</v>
       </c>
@@ -2705,7 +2683,7 @@
       <c r="S43" s="11"/>
       <c r="T43" s="11"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20">
       <c r="C44" s="11" t="s">
         <v>119</v>
       </c>
@@ -2731,7 +2709,7 @@
       <c r="S44" s="11"/>
       <c r="T44" s="11"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20">
       <c r="C45" s="11" t="s">
         <v>120</v>
       </c>
@@ -2759,7 +2737,7 @@
       <c r="S45" s="11"/>
       <c r="T45" s="11"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20">
       <c r="C46" s="5" t="s">
         <v>68</v>
       </c>
@@ -2781,11 +2759,11 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20">
       <c r="K48" s="9"/>
       <c r="M48" s="9"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
         <v>122</v>
@@ -2807,7 +2785,7 @@
       </c>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="A50" s="7" t="s">
         <v>126</v>
       </c>
@@ -2857,7 +2835,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="B51" s="1"/>
       <c r="C51" s="11" t="s">
         <v>93</v>
@@ -2884,7 +2862,7 @@
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="C52" s="11"/>
       <c r="D52" s="11" t="s">
         <v>141</v>
@@ -2906,7 +2884,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="C53" s="11"/>
       <c r="D53" s="11" t="s">
         <v>143</v>
@@ -2932,7 +2910,7 @@
       </c>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
         <v>148</v>
@@ -2954,7 +2932,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="C55" s="11"/>
       <c r="D55" s="11" t="s">
         <v>150</v>
@@ -2976,7 +2954,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="C56" s="11"/>
       <c r="D56" s="11" t="s">
         <v>152</v>
@@ -2998,7 +2976,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="C57" s="11"/>
       <c r="D57" s="11" t="s">
         <v>154</v>
@@ -3020,7 +2998,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
         <v>156</v>
@@ -3042,7 +3020,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="C59" s="11"/>
       <c r="D59" s="11" t="s">
         <v>158</v>
@@ -3064,7 +3042,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="C60" s="11"/>
       <c r="D60" s="11" t="s">
         <v>160</v>
@@ -3088,7 +3066,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="C61" s="11"/>
       <c r="D61" s="11" t="s">
         <v>164</v>
@@ -3112,7 +3090,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16">
       <c r="C62" s="11"/>
       <c r="D62" s="11" t="s">
         <v>166</v>
@@ -3136,7 +3114,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="C63" s="11"/>
       <c r="D63" s="11" t="s">
         <v>168</v>
@@ -3160,7 +3138,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="C64" s="11"/>
       <c r="D64" s="11" t="s">
         <v>170</v>
@@ -3184,7 +3162,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:16">
       <c r="C65" s="11"/>
       <c r="D65" s="11" t="s">
         <v>172</v>
@@ -3208,7 +3186,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:16">
       <c r="C66" s="11"/>
       <c r="D66" s="11" t="s">
         <v>174</v>
@@ -3230,7 +3208,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:16">
       <c r="C67" s="11"/>
       <c r="D67" s="11" t="s">
         <v>176</v>
@@ -3252,7 +3230,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:16">
       <c r="C68" s="11"/>
       <c r="D68" s="11" t="s">
         <v>178</v>
@@ -3274,7 +3252,7 @@
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
     </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:16">
       <c r="C69" s="11" t="s">
         <v>98</v>
       </c>
@@ -3300,7 +3278,7 @@
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
     </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:16">
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
         <v>182</v>
@@ -3326,7 +3304,7 @@
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
     </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:16">
       <c r="C71" s="11"/>
       <c r="D71" s="11" t="s">
         <v>186</v>
@@ -3350,7 +3328,7 @@
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
     </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:16">
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
         <v>189</v>
@@ -3376,7 +3354,7 @@
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
     </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:16">
       <c r="C73" s="11"/>
       <c r="D73" s="11" t="s">
         <v>192</v>
@@ -3400,7 +3378,7 @@
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
     </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:16">
       <c r="C74" s="11"/>
       <c r="D74" s="11" t="s">
         <v>194</v>
@@ -3424,7 +3402,7 @@
       <c r="O74" s="11"/>
       <c r="P74" s="11"/>
     </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:16">
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
         <v>197</v>
@@ -3450,7 +3428,7 @@
       <c r="O75" s="11"/>
       <c r="P75" s="11"/>
     </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:16">
       <c r="C76" s="11"/>
       <c r="D76" s="11" t="s">
         <v>201</v>
@@ -3474,7 +3452,7 @@
       <c r="O76" s="11"/>
       <c r="P76" s="11"/>
     </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:16">
       <c r="C77" s="11"/>
       <c r="D77" s="11" t="s">
         <v>204</v>
@@ -3498,7 +3476,7 @@
       <c r="O77" s="11"/>
       <c r="P77" s="11"/>
     </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:16">
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
         <v>206</v>
@@ -3524,7 +3502,7 @@
       <c r="O78" s="11"/>
       <c r="P78" s="11"/>
     </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:16">
       <c r="C79" s="11"/>
       <c r="D79" s="11" t="s">
         <v>209</v>
@@ -3548,7 +3526,7 @@
       <c r="O79" s="11"/>
       <c r="P79" s="11"/>
     </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:16">
       <c r="C80" s="11"/>
       <c r="D80" s="11" t="s">
         <v>212</v>
@@ -3572,7 +3550,7 @@
       <c r="O80" s="11"/>
       <c r="P80" s="11"/>
     </row>
-    <row r="81" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:16">
       <c r="C81" s="11"/>
       <c r="D81" s="11" t="s">
         <v>214</v>
@@ -3596,7 +3574,7 @@
       <c r="O81" s="11"/>
       <c r="P81" s="11"/>
     </row>
-    <row r="82" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:16">
       <c r="C82" s="11"/>
       <c r="D82" s="11" t="s">
         <v>217</v>
@@ -3620,7 +3598,7 @@
       <c r="O82" s="11"/>
       <c r="P82" s="11"/>
     </row>
-    <row r="83" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:16">
       <c r="C83" s="11" t="s">
         <v>105</v>
       </c>
@@ -3646,7 +3624,7 @@
       <c r="O83" s="11"/>
       <c r="P83" s="11"/>
     </row>
-    <row r="84" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:16">
       <c r="C84" s="11"/>
       <c r="D84" s="11" t="s">
         <v>224</v>
@@ -3672,7 +3650,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:16">
       <c r="C85" s="11"/>
       <c r="D85" s="11" t="s">
         <v>227</v>
@@ -3696,7 +3674,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:16">
       <c r="C86" s="11"/>
       <c r="D86" s="11" t="s">
         <v>229</v>
@@ -3720,7 +3698,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:16">
       <c r="C87" s="11"/>
       <c r="D87" s="11" t="s">
         <v>231</v>
@@ -3744,7 +3722,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:16">
       <c r="C88" s="11"/>
       <c r="D88" s="11" t="s">
         <v>234</v>
@@ -3770,7 +3748,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:16">
       <c r="C89" s="11"/>
       <c r="D89" s="11" t="s">
         <v>238</v>
@@ -3786,9 +3764,7 @@
       <c r="K89" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="L89" s="11" t="s">
-        <v>236</v>
-      </c>
+      <c r="L89" s="11"/>
       <c r="M89" s="11" t="s">
         <v>240</v>
       </c>
@@ -3796,7 +3772,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:16">
       <c r="C90" s="11"/>
       <c r="D90" s="11" t="s">
         <v>241</v>
@@ -3820,7 +3796,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:16">
       <c r="C91" s="11"/>
       <c r="D91" s="11" t="s">
         <v>244</v>
@@ -3848,7 +3824,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:16">
       <c r="C92" s="11"/>
       <c r="D92" s="11" t="s">
         <v>247</v>
@@ -3872,7 +3848,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:16">
       <c r="C93" s="11"/>
       <c r="D93" s="11" t="s">
         <v>249</v>
@@ -3898,7 +3874,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:16">
       <c r="C94" s="11"/>
       <c r="D94" s="11" t="s">
         <v>254</v>
@@ -3924,7 +3900,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:16">
       <c r="C95" s="11" t="s">
         <v>108</v>
       </c>
@@ -3950,7 +3926,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:16">
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
@@ -3976,7 +3952,7 @@
       </c>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:16">
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11" t="s">
@@ -4002,7 +3978,7 @@
       </c>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:16">
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
@@ -4028,7 +4004,7 @@
       </c>
       <c r="P98" s="11"/>
     </row>
-    <row r="99" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:16">
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11" t="s">
@@ -4054,7 +4030,7 @@
       </c>
       <c r="P99" s="11"/>
     </row>
-    <row r="100" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:16">
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11" t="s">
@@ -4082,7 +4058,7 @@
       </c>
       <c r="P100" s="11"/>
     </row>
-    <row r="101" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:16">
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
@@ -4106,7 +4082,7 @@
       <c r="O101" s="11"/>
       <c r="P101" s="11"/>
     </row>
-    <row r="102" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:16">
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
@@ -4132,7 +4108,7 @@
       </c>
       <c r="P102" s="11"/>
     </row>
-    <row r="103" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:16">
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
@@ -4158,7 +4134,7 @@
       </c>
       <c r="P103" s="11"/>
     </row>
-    <row r="104" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:16">
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
@@ -4184,7 +4160,7 @@
       </c>
       <c r="P104" s="11"/>
     </row>
-    <row r="105" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:16">
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11" t="s">
@@ -4210,7 +4186,7 @@
       </c>
       <c r="P105" s="11"/>
     </row>
-    <row r="106" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:16">
       <c r="C106" s="11"/>
       <c r="D106" s="11" t="s">
         <v>271</v>
@@ -4238,7 +4214,7 @@
       </c>
       <c r="P106" s="11"/>
     </row>
-    <row r="107" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:16">
       <c r="C107" s="11"/>
       <c r="D107" s="11" t="s">
         <v>275</v>
@@ -4264,7 +4240,7 @@
       </c>
       <c r="P107" s="11"/>
     </row>
-    <row r="108" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:16">
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11" t="s">
@@ -4292,7 +4268,7 @@
       </c>
       <c r="P108" s="11"/>
     </row>
-    <row r="109" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:16">
       <c r="C109" s="11"/>
       <c r="D109" s="11" t="s">
         <v>280</v>
@@ -4318,7 +4294,7 @@
       </c>
       <c r="P109" s="11"/>
     </row>
-    <row r="110" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:16">
       <c r="C110" s="11"/>
       <c r="D110" s="11" t="s">
         <v>283</v>
@@ -4344,7 +4320,7 @@
       </c>
       <c r="P110" s="11"/>
     </row>
-    <row r="111" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:16">
       <c r="C111" s="11" t="s">
         <v>110</v>
       </c>
@@ -4370,7 +4346,7 @@
       <c r="O111" s="11"/>
       <c r="P111" s="11"/>
     </row>
-    <row r="112" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:16">
       <c r="C112" s="11" t="s">
         <v>111</v>
       </c>
@@ -4396,7 +4372,7 @@
       <c r="O112" s="11"/>
       <c r="P112" s="11"/>
     </row>
-    <row r="113" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:16">
       <c r="C113" s="11"/>
       <c r="D113" s="11" t="s">
         <v>292</v>
@@ -4420,7 +4396,7 @@
       <c r="O113" s="11"/>
       <c r="P113" s="11"/>
     </row>
-    <row r="114" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:16">
       <c r="C114" s="11"/>
       <c r="D114" s="11" t="s">
         <v>295</v>
@@ -4444,7 +4420,7 @@
       <c r="O114" s="11"/>
       <c r="P114" s="11"/>
     </row>
-    <row r="115" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:16">
       <c r="C115" s="11"/>
       <c r="D115" s="11" t="s">
         <v>297</v>
@@ -4468,7 +4444,7 @@
       <c r="O115" s="11"/>
       <c r="P115" s="11"/>
     </row>
-    <row r="116" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:16">
       <c r="C116" s="11"/>
       <c r="D116" s="11" t="s">
         <v>300</v>
@@ -4492,7 +4468,7 @@
       <c r="O116" s="11"/>
       <c r="P116" s="11"/>
     </row>
-    <row r="117" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:16">
       <c r="C117" s="11"/>
       <c r="D117" s="11" t="s">
         <v>302</v>
@@ -4516,7 +4492,7 @@
       <c r="O117" s="11"/>
       <c r="P117" s="11"/>
     </row>
-    <row r="118" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:16">
       <c r="C118" s="11"/>
       <c r="D118" s="11" t="s">
         <v>305</v>
@@ -4540,7 +4516,7 @@
       <c r="O118" s="11"/>
       <c r="P118" s="11"/>
     </row>
-    <row r="119" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:16">
       <c r="C119" s="11"/>
       <c r="D119" s="11" t="s">
         <v>308</v>
@@ -4564,7 +4540,7 @@
       <c r="O119" s="11"/>
       <c r="P119" s="11"/>
     </row>
-    <row r="120" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:16">
       <c r="C120" s="11" t="s">
         <v>113</v>
       </c>
@@ -4592,7 +4568,7 @@
       <c r="O120" s="11"/>
       <c r="P120" s="11"/>
     </row>
-    <row r="121" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:16">
       <c r="C121" s="11"/>
       <c r="D121" s="11" t="s">
         <v>292</v>
@@ -4618,7 +4594,7 @@
       <c r="O121" s="11"/>
       <c r="P121" s="11"/>
     </row>
-    <row r="122" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:16">
       <c r="C122" s="11"/>
       <c r="D122" s="11" t="s">
         <v>315</v>
@@ -4644,7 +4620,7 @@
       <c r="O122" s="11"/>
       <c r="P122" s="11"/>
     </row>
-    <row r="123" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:16">
       <c r="C123" s="11"/>
       <c r="D123" s="11" t="s">
         <v>308</v>
@@ -4670,7 +4646,7 @@
       <c r="O123" s="11"/>
       <c r="P123" s="11"/>
     </row>
-    <row r="124" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:16">
       <c r="C124" s="11" t="s">
         <v>115</v>
       </c>
@@ -4700,7 +4676,7 @@
       <c r="O124" s="11"/>
       <c r="P124" s="11"/>
     </row>
-    <row r="125" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:16">
       <c r="C125" s="11"/>
       <c r="D125" s="11" t="s">
         <v>322</v>
@@ -4726,7 +4702,7 @@
       <c r="O125" s="11"/>
       <c r="P125" s="11"/>
     </row>
-    <row r="126" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:16">
       <c r="C126" s="11"/>
       <c r="D126" s="11" t="s">
         <v>323</v>
@@ -4754,7 +4730,7 @@
       <c r="O126" s="11"/>
       <c r="P126" s="11"/>
     </row>
-    <row r="127" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:16">
       <c r="C127" s="11"/>
       <c r="D127" s="11" t="s">
         <v>326</v>
@@ -4782,7 +4758,7 @@
       <c r="O127" s="11"/>
       <c r="P127" s="11"/>
     </row>
-    <row r="128" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:16">
       <c r="C128" s="11"/>
       <c r="D128" s="11" t="s">
         <v>329</v>
@@ -4806,7 +4782,7 @@
       <c r="O128" s="11"/>
       <c r="P128" s="11"/>
     </row>
-    <row r="129" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:16">
       <c r="C129" s="11" t="s">
         <v>117</v>
       </c>
@@ -4834,7 +4810,7 @@
       <c r="O129" s="11"/>
       <c r="P129" s="11"/>
     </row>
-    <row r="130" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:16">
       <c r="C130" s="11"/>
       <c r="D130" s="11" t="s">
         <v>337</v>
@@ -4860,7 +4836,7 @@
       <c r="O130" s="11"/>
       <c r="P130" s="11"/>
     </row>
-    <row r="131" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:16">
       <c r="C131" s="11"/>
       <c r="D131" s="11" t="s">
         <v>341</v>
@@ -4886,7 +4862,7 @@
       <c r="O131" s="11"/>
       <c r="P131" s="11"/>
     </row>
-    <row r="132" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:16">
       <c r="C132" s="11"/>
       <c r="D132" s="11" t="s">
         <v>345</v>
@@ -4912,7 +4888,7 @@
       <c r="O132" s="11"/>
       <c r="P132" s="11"/>
     </row>
-    <row r="133" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:16">
       <c r="C133" s="11" t="s">
         <v>119</v>
       </c>
@@ -4940,7 +4916,7 @@
       <c r="O133" s="11"/>
       <c r="P133" s="11"/>
     </row>
-    <row r="134" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:16">
       <c r="C134" s="11"/>
       <c r="D134" s="11" t="s">
         <v>353</v>
@@ -4966,7 +4942,7 @@
       <c r="O134" s="11"/>
       <c r="P134" s="11"/>
     </row>
-    <row r="135" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:16">
       <c r="C135" s="11"/>
       <c r="D135" s="11" t="s">
         <v>357</v>
@@ -4992,7 +4968,7 @@
       <c r="O135" s="11"/>
       <c r="P135" s="11"/>
     </row>
-    <row r="136" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:16">
       <c r="C136" s="11"/>
       <c r="D136" s="11" t="s">
         <v>361</v>
@@ -5018,7 +4994,7 @@
       <c r="O136" s="11"/>
       <c r="P136" s="11"/>
     </row>
-    <row r="137" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:16">
       <c r="C137" s="11"/>
       <c r="D137" s="11" t="s">
         <v>365</v>
@@ -5044,7 +5020,7 @@
       <c r="O137" s="11"/>
       <c r="P137" s="11"/>
     </row>
-    <row r="138" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:16">
       <c r="C138" s="11"/>
       <c r="D138" s="11" t="s">
         <v>369</v>
@@ -5070,7 +5046,7 @@
       <c r="O138" s="11"/>
       <c r="P138" s="11"/>
     </row>
-    <row r="139" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:16">
       <c r="C139" s="11"/>
       <c r="D139" s="11" t="s">
         <v>373</v>
@@ -5096,7 +5072,7 @@
       <c r="O139" s="11"/>
       <c r="P139" s="11"/>
     </row>
-    <row r="140" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:16">
       <c r="C140" s="11"/>
       <c r="D140" s="11" t="s">
         <v>376</v>
@@ -5122,7 +5098,7 @@
       <c r="O140" s="11"/>
       <c r="P140" s="11"/>
     </row>
-    <row r="141" spans="3:16" ht="120" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:16">
       <c r="C141" s="11"/>
       <c r="D141" s="11" t="s">
         <v>379</v>
@@ -5138,7 +5114,7 @@
       <c r="K141" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="L141" s="19" t="s">
+      <c r="L141" s="11" t="s">
         <v>381</v>
       </c>
       <c r="M141" s="11"/>
@@ -5148,7 +5124,7 @@
       <c r="O141" s="11"/>
       <c r="P141" s="11"/>
     </row>
-    <row r="142" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:16">
       <c r="C142" s="11"/>
       <c r="D142" s="11" t="s">
         <v>383</v>
@@ -5174,7 +5150,7 @@
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
     </row>
-    <row r="143" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:16">
       <c r="C143" s="11" t="s">
         <v>120</v>
       </c>
@@ -5198,7 +5174,7 @@
       <c r="O143" s="11"/>
       <c r="P143" s="11"/>
     </row>
-    <row r="144" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:16">
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
@@ -5220,7 +5196,7 @@
       <c r="O144" s="11"/>
       <c r="P144" s="11"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16">
       <c r="C145" s="11"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11" t="s">
@@ -5242,7 +5218,7 @@
       <c r="O145" s="11"/>
       <c r="P145" s="11"/>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16">
       <c r="C146" s="11"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11" t="s">
@@ -5264,7 +5240,7 @@
       <c r="O146" s="11"/>
       <c r="P146" s="11"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16">
       <c r="C147" s="5" t="s">
         <v>68</v>
       </c>
@@ -5282,7 +5258,7 @@
       <c r="O147" s="3"/>
       <c r="P147" s="3"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16">
       <c r="A151" s="7" t="s">
         <v>390</v>
       </c>
@@ -5299,22 +5275,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16">
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16">
       <c r="C153" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16">
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16">
       <c r="A157" s="7" t="s">
         <v>393</v>
       </c>
@@ -5337,14 +5313,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16">
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
       <c r="G158" s="11"/>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16">
       <c r="C159" s="5" t="s">
         <v>68</v>
       </c>
@@ -5353,7 +5329,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11">
       <c r="B162" s="16" t="s">
         <v>398</v>
       </c>
@@ -5361,7 +5337,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11">
       <c r="A163" s="12" t="s">
         <v>400</v>
       </c>
@@ -5391,7 +5367,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11">
       <c r="C164" s="11" t="s">
         <v>98</v>
       </c>
@@ -5409,7 +5385,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11">
       <c r="C165" s="11"/>
       <c r="D165" s="11" t="s">
         <v>182</v>
@@ -5422,7 +5398,7 @@
       <c r="H165" s="11"/>
       <c r="I165" s="11"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11">
       <c r="C166" s="11"/>
       <c r="D166" s="11" t="s">
         <v>186</v>
@@ -5435,7 +5411,7 @@
       <c r="H166" s="11"/>
       <c r="I166" s="11"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11">
       <c r="C167" s="11"/>
       <c r="D167" s="11" t="s">
         <v>189</v>
@@ -5448,7 +5424,7 @@
       <c r="H167" s="11"/>
       <c r="I167" s="11"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11">
       <c r="C168" s="11"/>
       <c r="D168" s="11" t="s">
         <v>192</v>
@@ -5461,7 +5437,7 @@
       <c r="H168" s="11"/>
       <c r="I168" s="11"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11">
       <c r="C169" s="11"/>
       <c r="D169" s="11" t="s">
         <v>194</v>
@@ -5476,7 +5452,7 @@
       <c r="H169" s="11"/>
       <c r="I169" s="11"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11">
       <c r="C170" s="11"/>
       <c r="D170" s="11" t="s">
         <v>197</v>
@@ -5489,7 +5465,7 @@
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11">
       <c r="C171" s="11"/>
       <c r="D171" s="11" t="s">
         <v>201</v>
@@ -5502,7 +5478,7 @@
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11">
       <c r="C172" s="11"/>
       <c r="D172" s="11" t="s">
         <v>204</v>
@@ -5517,7 +5493,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="11"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11">
       <c r="C173" s="11"/>
       <c r="D173" s="11" t="s">
         <v>206</v>
@@ -5530,7 +5506,7 @@
       <c r="H173" s="11"/>
       <c r="I173" s="11"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11">
       <c r="C174" s="11"/>
       <c r="D174" s="11" t="s">
         <v>209</v>
@@ -5545,7 +5521,7 @@
       <c r="H174" s="11"/>
       <c r="I174" s="11"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11">
       <c r="C175" s="11"/>
       <c r="D175" s="11" t="s">
         <v>212</v>
@@ -5558,7 +5534,7 @@
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11">
       <c r="C176" s="11"/>
       <c r="D176" s="11" t="s">
         <v>214</v>
@@ -5571,7 +5547,7 @@
       <c r="H176" s="11"/>
       <c r="I176" s="11"/>
     </row>
-    <row r="177" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:9">
       <c r="C177" s="11" t="s">
         <v>111</v>
       </c>
@@ -5586,7 +5562,7 @@
       <c r="H177" s="11"/>
       <c r="I177" s="11"/>
     </row>
-    <row r="178" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:9">
       <c r="C178" s="11"/>
       <c r="D178" s="11" t="s">
         <v>292</v>
@@ -5599,7 +5575,7 @@
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
     </row>
-    <row r="179" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:9">
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
         <v>295</v>
@@ -5612,7 +5588,7 @@
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
     </row>
-    <row r="180" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:9">
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
         <v>297</v>
@@ -5627,7 +5603,7 @@
       </c>
       <c r="I180" s="11"/>
     </row>
-    <row r="181" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:9">
       <c r="C181" s="11"/>
       <c r="D181" s="11" t="s">
         <v>300</v>
@@ -5642,7 +5618,7 @@
       </c>
       <c r="I181" s="11"/>
     </row>
-    <row r="182" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:9">
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
         <v>302</v>
@@ -5657,7 +5633,7 @@
       </c>
       <c r="I182" s="11"/>
     </row>
-    <row r="183" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:9">
       <c r="C183" s="11"/>
       <c r="D183" s="11" t="s">
         <v>305</v>
@@ -5672,7 +5648,7 @@
       </c>
       <c r="I183" s="11"/>
     </row>
-    <row r="184" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:9">
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
         <v>308</v>
@@ -5687,7 +5663,7 @@
       </c>
       <c r="I184" s="11"/>
     </row>
-    <row r="185" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:9">
       <c r="C185" s="11" t="s">
         <v>113</v>
       </c>
@@ -5702,7 +5678,7 @@
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
     </row>
-    <row r="186" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:9">
       <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
         <v>292</v>
@@ -5715,7 +5691,7 @@
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
     </row>
-    <row r="187" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:9">
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
         <v>315</v>
@@ -5730,7 +5706,7 @@
       </c>
       <c r="I187" s="11"/>
     </row>
-    <row r="188" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:9">
       <c r="C188" s="11"/>
       <c r="D188" s="11" t="s">
         <v>308</v>
@@ -5745,7 +5721,7 @@
       </c>
       <c r="I188" s="11"/>
     </row>
-    <row r="189" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:9">
       <c r="C189" s="11" t="s">
         <v>115</v>
       </c>
@@ -5760,7 +5736,7 @@
       <c r="H189" s="11"/>
       <c r="I189" s="11"/>
     </row>
-    <row r="190" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:9">
       <c r="C190" s="11"/>
       <c r="D190" s="11" t="s">
         <v>322</v>
@@ -5775,7 +5751,7 @@
       </c>
       <c r="I190" s="11"/>
     </row>
-    <row r="191" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:9">
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
         <v>323</v>
@@ -5790,7 +5766,7 @@
       </c>
       <c r="I191" s="11"/>
     </row>
-    <row r="192" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:9">
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
         <v>326</v>
@@ -5805,7 +5781,7 @@
       </c>
       <c r="I192" s="11"/>
     </row>
-    <row r="193" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:9">
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
         <v>329</v>
@@ -5820,7 +5796,7 @@
       </c>
       <c r="I193" s="11"/>
     </row>
-    <row r="194" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:9">
       <c r="C194" s="5" t="s">
         <v>68</v>
       </c>
@@ -5831,7 +5807,7 @@
       <c r="H194" s="3"/>
       <c r="I194" s="3"/>
     </row>
-    <row r="195" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:9">
       <c r="H195" s="8"/>
     </row>
   </sheetData>
@@ -5842,20 +5818,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A5:C32"/>
   <sheetViews>
@@ -5863,12 +5839,12 @@
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5876,12 +5852,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Bugfix: Fixed an issue with the calculation precision in the summary row of the table.
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES005.xlsx
+++ b/apps/es/resources/screen/ES005.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="414">
   <si>
     <t>Do not modify this column</t>
   </si>
@@ -749,9 +749,6 @@
   </si>
   <si>
     <t>Amount</t>
-  </si>
-  <si>
-    <t>format: #,###.00</t>
   </si>
   <si>
     <t>amt</t>
@@ -1036,6 +1033,9 @@
   </si>
   <si>
     <t>This Prior Balance</t>
+  </si>
+  <si>
+    <t>format: #,###.00</t>
   </si>
   <si>
     <t>deduction_amt</t>
@@ -1295,7 +1295,7 @@
     <t>One tailor made javascript for each layout</t>
   </si>
   <si>
-    <t>20250529092300</t>
+    <t>20250529111700</t>
   </si>
 </sst>
 </file>
@@ -3738,11 +3738,9 @@
       <c r="K88" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="L88" s="11" t="s">
+      <c r="L88" s="11"/>
+      <c r="M88" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="M88" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="N88" s="11"/>
       <c r="O88" s="11"/>
@@ -3751,10 +3749,10 @@
     <row r="89" spans="3:16">
       <c r="C89" s="11"/>
       <c r="D89" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E89" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
@@ -3766,7 +3764,7 @@
       </c>
       <c r="L89" s="11"/>
       <c r="M89" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N89" s="11"/>
       <c r="O89" s="11"/>
@@ -3775,10 +3773,10 @@
     <row r="90" spans="3:16">
       <c r="C90" s="11"/>
       <c r="D90" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
@@ -3790,7 +3788,7 @@
       </c>
       <c r="L90" s="11"/>
       <c r="M90" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N90" s="11"/>
       <c r="O90" s="11"/>
@@ -3799,13 +3797,13 @@
     <row r="91" spans="3:16">
       <c r="C91" s="11"/>
       <c r="D91" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>235</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -3814,11 +3812,9 @@
       <c r="K91" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="L91" s="11" t="s">
-        <v>236</v>
-      </c>
+      <c r="L91" s="11"/>
       <c r="M91" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N91" s="11"/>
       <c r="O91" s="11"/>
@@ -3827,7 +3823,7 @@
     <row r="92" spans="3:16">
       <c r="C92" s="11"/>
       <c r="D92" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>177</v>
@@ -3842,7 +3838,7 @@
       </c>
       <c r="L92" s="11"/>
       <c r="M92" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N92" s="11"/>
       <c r="O92" s="11"/>
@@ -3851,7 +3847,7 @@
     <row r="93" spans="3:16">
       <c r="C93" s="11"/>
       <c r="D93" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
@@ -3860,16 +3856,16 @@
       <c r="I93" s="11"/>
       <c r="J93" s="11"/>
       <c r="K93" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="L93" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="L93" s="11" t="s">
+      <c r="M93" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="M93" s="11" t="s">
+      <c r="N93" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="N93" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
@@ -3877,7 +3873,7 @@
     <row r="94" spans="3:16">
       <c r="C94" s="11"/>
       <c r="D94" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
@@ -3886,16 +3882,16 @@
       <c r="I94" s="11"/>
       <c r="J94" s="11"/>
       <c r="K94" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L94" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="M94" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="M94" s="11" t="s">
+      <c r="N94" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="N94" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
@@ -3911,7 +3907,7 @@
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I95" s="11"/>
       <c r="J95" s="11"/>
@@ -3935,7 +3931,7 @@
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I96" s="11"/>
       <c r="J96" s="11"/>
@@ -3948,7 +3944,7 @@
       </c>
       <c r="N96" s="11"/>
       <c r="O96" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P96" s="11"/>
     </row>
@@ -3961,7 +3957,7 @@
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I97" s="11"/>
       <c r="J97" s="11"/>
@@ -3974,7 +3970,7 @@
       </c>
       <c r="N97" s="11"/>
       <c r="O97" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P97" s="11"/>
     </row>
@@ -3982,25 +3978,25 @@
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F98" s="11"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I98" s="11"/>
       <c r="J98" s="11"/>
       <c r="K98" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L98" s="11"/>
       <c r="M98" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N98" s="11"/>
       <c r="O98" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P98" s="11"/>
     </row>
@@ -4008,12 +4004,12 @@
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
       <c r="H99" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I99" s="11"/>
       <c r="J99" s="11"/>
@@ -4026,7 +4022,7 @@
       </c>
       <c r="N99" s="11"/>
       <c r="O99" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P99" s="11"/>
     </row>
@@ -4034,14 +4030,14 @@
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F100" s="11"/>
       <c r="G100" s="11" t="s">
         <v>30</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I100" s="11"/>
       <c r="J100" s="11"/>
@@ -4050,11 +4046,11 @@
       </c>
       <c r="L100" s="11"/>
       <c r="M100" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N100" s="11"/>
       <c r="O100" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P100" s="11"/>
     </row>
@@ -4062,21 +4058,21 @@
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F101" s="11"/>
       <c r="G101" s="11"/>
       <c r="H101" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I101" s="11"/>
       <c r="J101" s="11"/>
       <c r="K101" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L101" s="11"/>
       <c r="M101" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N101" s="11"/>
       <c r="O101" s="11"/>
@@ -4086,12 +4082,12 @@
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11"/>
       <c r="H102" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I102" s="11"/>
       <c r="J102" s="11"/>
@@ -4104,7 +4100,7 @@
       </c>
       <c r="N102" s="11"/>
       <c r="O102" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P102" s="11"/>
     </row>
@@ -4112,12 +4108,12 @@
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="11"/>
       <c r="H103" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I103" s="11"/>
       <c r="J103" s="11"/>
@@ -4130,7 +4126,7 @@
       </c>
       <c r="N103" s="11"/>
       <c r="O103" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P103" s="11"/>
     </row>
@@ -4143,12 +4139,12 @@
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
       <c r="H104" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I104" s="11"/>
       <c r="J104" s="11"/>
       <c r="K104" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L104" s="11"/>
       <c r="M104" s="11" t="s">
@@ -4156,7 +4152,7 @@
       </c>
       <c r="N104" s="11"/>
       <c r="O104" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P104" s="11"/>
     </row>
@@ -4169,7 +4165,7 @@
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
       <c r="H105" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I105" s="11"/>
       <c r="J105" s="11"/>
@@ -4182,17 +4178,17 @@
       </c>
       <c r="N105" s="11"/>
       <c r="O105" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P105" s="11"/>
     </row>
     <row r="106" spans="3:16">
       <c r="C106" s="11"/>
       <c r="D106" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>272</v>
       </c>
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
@@ -4203,24 +4199,24 @@
         <v>145</v>
       </c>
       <c r="L106" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="M106" s="11" t="s">
         <v>273</v>
-      </c>
-      <c r="M106" s="11" t="s">
-        <v>274</v>
       </c>
       <c r="N106" s="11"/>
       <c r="O106" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P106" s="11"/>
     </row>
     <row r="107" spans="3:16">
       <c r="C107" s="11"/>
       <c r="D107" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>276</v>
       </c>
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
@@ -4232,11 +4228,11 @@
       </c>
       <c r="L107" s="11"/>
       <c r="M107" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N107" s="11"/>
       <c r="O107" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P107" s="11"/>
     </row>
@@ -4244,12 +4240,12 @@
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F108" s="11"/>
       <c r="G108" s="11"/>
       <c r="H108" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
@@ -4260,21 +4256,21 @@
         <v>199</v>
       </c>
       <c r="M108" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N108" s="11"/>
       <c r="O108" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P108" s="11"/>
     </row>
     <row r="109" spans="3:16">
       <c r="C109" s="11"/>
       <c r="D109" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E109" s="11" t="s">
         <v>280</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>281</v>
       </c>
       <c r="F109" s="11"/>
       <c r="G109" s="11"/>
@@ -4286,21 +4282,21 @@
       </c>
       <c r="L109" s="11"/>
       <c r="M109" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N109" s="11"/>
       <c r="O109" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P109" s="11"/>
     </row>
     <row r="110" spans="3:16">
       <c r="C110" s="11"/>
       <c r="D110" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="E110" s="11" t="s">
         <v>283</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>284</v>
       </c>
       <c r="F110" s="11"/>
       <c r="G110" s="11"/>
@@ -4312,11 +4308,11 @@
       </c>
       <c r="L110" s="11"/>
       <c r="M110" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N110" s="11"/>
       <c r="O110" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P110" s="11"/>
     </row>
@@ -4325,10 +4321,10 @@
         <v>110</v>
       </c>
       <c r="D111" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E111" s="11" t="s">
         <v>285</v>
-      </c>
-      <c r="E111" s="11" t="s">
-        <v>286</v>
       </c>
       <c r="F111" s="11"/>
       <c r="G111" s="11"/>
@@ -4336,10 +4332,10 @@
       <c r="I111" s="11"/>
       <c r="J111" s="11"/>
       <c r="K111" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="L111" s="11" t="s">
         <v>287</v>
-      </c>
-      <c r="L111" s="11" t="s">
-        <v>288</v>
       </c>
       <c r="M111" s="11"/>
       <c r="N111" s="11"/>
@@ -4351,10 +4347,10 @@
         <v>111</v>
       </c>
       <c r="D112" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="E112" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="F112" s="11"/>
       <c r="G112" s="11"/>
@@ -4366,7 +4362,7 @@
       </c>
       <c r="L112" s="11"/>
       <c r="M112" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N112" s="11"/>
       <c r="O112" s="11"/>
@@ -4375,10 +4371,10 @@
     <row r="113" spans="3:16">
       <c r="C113" s="11"/>
       <c r="D113" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>292</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>293</v>
       </c>
       <c r="F113" s="11"/>
       <c r="G113" s="11"/>
@@ -4390,7 +4386,7 @@
       </c>
       <c r="L113" s="11"/>
       <c r="M113" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N113" s="11"/>
       <c r="O113" s="11"/>
@@ -4399,7 +4395,7 @@
     <row r="114" spans="3:16">
       <c r="C114" s="11"/>
       <c r="D114" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E114" s="11" t="s">
         <v>232</v>
@@ -4414,7 +4410,7 @@
       </c>
       <c r="L114" s="11"/>
       <c r="M114" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N114" s="11"/>
       <c r="O114" s="11"/>
@@ -4423,10 +4419,10 @@
     <row r="115" spans="3:16">
       <c r="C115" s="11"/>
       <c r="D115" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="E115" s="11" t="s">
         <v>297</v>
-      </c>
-      <c r="E115" s="11" t="s">
-        <v>298</v>
       </c>
       <c r="F115" s="11"/>
       <c r="G115" s="11"/>
@@ -4438,7 +4434,7 @@
       </c>
       <c r="L115" s="11"/>
       <c r="M115" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N115" s="11"/>
       <c r="O115" s="11"/>
@@ -4447,10 +4443,10 @@
     <row r="116" spans="3:16">
       <c r="C116" s="11"/>
       <c r="D116" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="E116" s="11" t="s">
         <v>300</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>301</v>
       </c>
       <c r="F116" s="11"/>
       <c r="G116" s="11"/>
@@ -4462,7 +4458,7 @@
       </c>
       <c r="L116" s="11"/>
       <c r="M116" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N116" s="11"/>
       <c r="O116" s="11"/>
@@ -4471,10 +4467,10 @@
     <row r="117" spans="3:16">
       <c r="C117" s="11"/>
       <c r="D117" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E117" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="E117" s="11" t="s">
-        <v>303</v>
       </c>
       <c r="F117" s="11"/>
       <c r="G117" s="11"/>
@@ -4486,7 +4482,7 @@
       </c>
       <c r="L117" s="11"/>
       <c r="M117" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N117" s="11"/>
       <c r="O117" s="11"/>
@@ -4495,10 +4491,10 @@
     <row r="118" spans="3:16">
       <c r="C118" s="11"/>
       <c r="D118" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E118" s="11" t="s">
         <v>305</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>306</v>
       </c>
       <c r="F118" s="11"/>
       <c r="G118" s="11"/>
@@ -4510,7 +4506,7 @@
       </c>
       <c r="L118" s="11"/>
       <c r="M118" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N118" s="11"/>
       <c r="O118" s="11"/>
@@ -4519,10 +4515,10 @@
     <row r="119" spans="3:16">
       <c r="C119" s="11"/>
       <c r="D119" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="E119" s="11" t="s">
         <v>308</v>
-      </c>
-      <c r="E119" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="F119" s="11"/>
       <c r="G119" s="11"/>
@@ -4534,7 +4530,7 @@
       </c>
       <c r="L119" s="11"/>
       <c r="M119" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N119" s="11"/>
       <c r="O119" s="11"/>
@@ -4545,15 +4541,15 @@
         <v>113</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F120" s="11"/>
       <c r="G120" s="11"/>
       <c r="H120" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I120" s="11"/>
       <c r="J120" s="11"/>
@@ -4562,7 +4558,7 @@
       </c>
       <c r="L120" s="11"/>
       <c r="M120" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N120" s="11"/>
       <c r="O120" s="11"/>
@@ -4571,15 +4567,15 @@
     <row r="121" spans="3:16">
       <c r="C121" s="11"/>
       <c r="D121" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F121" s="11"/>
       <c r="G121" s="11"/>
       <c r="H121" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I121" s="11"/>
       <c r="J121" s="11"/>
@@ -4588,7 +4584,7 @@
       </c>
       <c r="L121" s="11"/>
       <c r="M121" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N121" s="11"/>
       <c r="O121" s="11"/>
@@ -4597,7 +4593,7 @@
     <row r="122" spans="3:16">
       <c r="C122" s="11"/>
       <c r="D122" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>232</v>
@@ -4605,7 +4601,7 @@
       <c r="F122" s="11"/>
       <c r="G122" s="11"/>
       <c r="H122" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I122" s="11"/>
       <c r="J122" s="11"/>
@@ -4614,7 +4610,7 @@
       </c>
       <c r="L122" s="11"/>
       <c r="M122" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N122" s="11"/>
       <c r="O122" s="11"/>
@@ -4623,15 +4619,15 @@
     <row r="123" spans="3:16">
       <c r="C123" s="11"/>
       <c r="D123" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F123" s="11"/>
       <c r="G123" s="11"/>
       <c r="H123" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I123" s="11"/>
       <c r="J123" s="11"/>
@@ -4640,7 +4636,7 @@
       </c>
       <c r="L123" s="11"/>
       <c r="M123" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N123" s="11"/>
       <c r="O123" s="11"/>
@@ -4651,17 +4647,17 @@
         <v>115</v>
       </c>
       <c r="D124" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E124" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="E124" s="11" t="s">
-        <v>320</v>
-      </c>
       <c r="F124" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G124" s="11"/>
       <c r="H124" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I124" s="11"/>
       <c r="J124" s="11"/>
@@ -4670,7 +4666,7 @@
       </c>
       <c r="L124" s="11"/>
       <c r="M124" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N124" s="11"/>
       <c r="O124" s="11"/>
@@ -4679,7 +4675,7 @@
     <row r="125" spans="3:16">
       <c r="C125" s="11"/>
       <c r="D125" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>232</v>
@@ -4687,7 +4683,7 @@
       <c r="F125" s="11"/>
       <c r="G125" s="11"/>
       <c r="H125" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I125" s="11"/>
       <c r="J125" s="11"/>
@@ -4705,17 +4701,17 @@
     <row r="126" spans="3:16">
       <c r="C126" s="11"/>
       <c r="D126" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E126" s="11" t="s">
         <v>235</v>
       </c>
       <c r="F126" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G126" s="11"/>
       <c r="H126" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I126" s="11"/>
       <c r="J126" s="11"/>
@@ -4724,7 +4720,7 @@
       </c>
       <c r="L126" s="11"/>
       <c r="M126" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N126" s="11"/>
       <c r="O126" s="11"/>
@@ -4733,17 +4729,17 @@
     <row r="127" spans="3:16">
       <c r="C127" s="11"/>
       <c r="D127" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E127" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="E127" s="11" t="s">
+      <c r="F127" s="11" t="s">
         <v>327</v>
-      </c>
-      <c r="F127" s="11" t="s">
-        <v>328</v>
       </c>
       <c r="G127" s="11"/>
       <c r="H127" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I127" s="11"/>
       <c r="J127" s="11"/>
@@ -4752,7 +4748,7 @@
       </c>
       <c r="L127" s="11"/>
       <c r="M127" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N127" s="11"/>
       <c r="O127" s="11"/>
@@ -4761,10 +4757,10 @@
     <row r="128" spans="3:16">
       <c r="C128" s="11"/>
       <c r="D128" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E128" s="11" t="s">
         <v>329</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>330</v>
       </c>
       <c r="F128" s="11"/>
       <c r="G128" s="11"/>
@@ -4774,7 +4770,9 @@
       <c r="K128" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="L128" s="11"/>
+      <c r="L128" s="11" t="s">
+        <v>330</v>
+      </c>
       <c r="M128" s="11" t="s">
         <v>331</v>
       </c>
@@ -5089,7 +5087,7 @@
         <v>334</v>
       </c>
       <c r="L140" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M140" s="11"/>
       <c r="N140" s="11" t="s">
@@ -5161,7 +5159,7 @@
       <c r="F143" s="11"/>
       <c r="G143" s="11"/>
       <c r="H143" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I143" s="11"/>
       <c r="J143" s="11"/>
@@ -5183,7 +5181,7 @@
       <c r="F144" s="11"/>
       <c r="G144" s="11"/>
       <c r="H144" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I144" s="11"/>
       <c r="J144" s="11"/>
@@ -5205,7 +5203,7 @@
       <c r="F145" s="11"/>
       <c r="G145" s="11"/>
       <c r="H145" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I145" s="11"/>
       <c r="J145" s="11"/>
@@ -5227,7 +5225,7 @@
       <c r="F146" s="11"/>
       <c r="G146" s="11"/>
       <c r="H146" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I146" s="11"/>
       <c r="J146" s="11"/>
@@ -5552,10 +5550,10 @@
         <v>111</v>
       </c>
       <c r="D177" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="E177" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="E177" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="F177" s="11"/>
       <c r="G177" s="11"/>
@@ -5565,10 +5563,10 @@
     <row r="178" spans="3:9">
       <c r="C178" s="11"/>
       <c r="D178" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E178" s="11" t="s">
         <v>292</v>
-      </c>
-      <c r="E178" s="11" t="s">
-        <v>293</v>
       </c>
       <c r="F178" s="11"/>
       <c r="G178" s="11"/>
@@ -5578,7 +5576,7 @@
     <row r="179" spans="3:9">
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>232</v>
@@ -5591,10 +5589,10 @@
     <row r="180" spans="3:9">
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="E180" s="11" t="s">
         <v>297</v>
-      </c>
-      <c r="E180" s="11" t="s">
-        <v>298</v>
       </c>
       <c r="F180" s="11"/>
       <c r="G180" s="11"/>
@@ -5606,10 +5604,10 @@
     <row r="181" spans="3:9">
       <c r="C181" s="11"/>
       <c r="D181" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="E181" s="11" t="s">
         <v>300</v>
-      </c>
-      <c r="E181" s="11" t="s">
-        <v>301</v>
       </c>
       <c r="F181" s="11"/>
       <c r="G181" s="11"/>
@@ -5621,10 +5619,10 @@
     <row r="182" spans="3:9">
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E182" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="E182" s="11" t="s">
-        <v>303</v>
       </c>
       <c r="F182" s="11"/>
       <c r="G182" s="11"/>
@@ -5636,10 +5634,10 @@
     <row r="183" spans="3:9">
       <c r="C183" s="11"/>
       <c r="D183" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E183" s="11" t="s">
         <v>305</v>
-      </c>
-      <c r="E183" s="11" t="s">
-        <v>306</v>
       </c>
       <c r="F183" s="11"/>
       <c r="G183" s="11"/>
@@ -5651,10 +5649,10 @@
     <row r="184" spans="3:9">
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="E184" s="11" t="s">
         <v>308</v>
-      </c>
-      <c r="E184" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="F184" s="11"/>
       <c r="G184" s="11"/>
@@ -5668,10 +5666,10 @@
         <v>113</v>
       </c>
       <c r="D185" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E185" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F185" s="11"/>
       <c r="G185" s="11"/>
@@ -5681,10 +5679,10 @@
     <row r="186" spans="3:9">
       <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E186" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F186" s="11"/>
       <c r="G186" s="11"/>
@@ -5694,7 +5692,7 @@
     <row r="187" spans="3:9">
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E187" s="11" t="s">
         <v>232</v>
@@ -5709,10 +5707,10 @@
     <row r="188" spans="3:9">
       <c r="C188" s="11"/>
       <c r="D188" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E188" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F188" s="11"/>
       <c r="G188" s="11"/>
@@ -5726,10 +5724,10 @@
         <v>115</v>
       </c>
       <c r="D189" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E189" s="11" t="s">
         <v>319</v>
-      </c>
-      <c r="E189" s="11" t="s">
-        <v>320</v>
       </c>
       <c r="F189" s="11"/>
       <c r="G189" s="11"/>
@@ -5739,7 +5737,7 @@
     <row r="190" spans="3:9">
       <c r="C190" s="11"/>
       <c r="D190" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E190" s="11" t="s">
         <v>232</v>
@@ -5754,7 +5752,7 @@
     <row r="191" spans="3:9">
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>235</v>
@@ -5769,10 +5767,10 @@
     <row r="192" spans="3:9">
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E192" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="E192" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="F192" s="11"/>
       <c r="G192" s="11"/>
@@ -5784,10 +5782,10 @@
     <row r="193" spans="3:9">
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E193" s="11" t="s">
         <v>329</v>
-      </c>
-      <c r="E193" s="11" t="s">
-        <v>330</v>
       </c>
       <c r="F193" s="11"/>
       <c r="G193" s="11"/>

</xml_diff>

<commit_message>
Modified app/es: 1) Bugfix. 2) Modify ES101 - Expense Report. 3) Add ES102 - Cash Advancement Report
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES005.xlsx
+++ b/apps/es/resources/screen/ES005.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-1005" yWindow="-105" windowWidth="29040" windowHeight="4170"/>
@@ -12,7 +12,6 @@
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1146,16 +1145,6 @@
     <t>approve(hdrFg)</t>
   </si>
   <si>
-    <t>bttSubmitPettyCashExpense</t>
-  </si>
-  <si>
-    <t>Submit this petty cash expense to accounting</t>
-  </si>
-  <si>
-    <t>icon:images/action_button.gif
-dialog:content: Are you sure to submit this petty cash expense to accounting for final approval?</t>
-  </si>
-  <si>
     <t>submitPettyCashExpense(settleByPriorBalanceDetailFg)</t>
   </si>
   <si>
@@ -1295,14 +1284,24 @@
     <t>One tailor made javascript for each layout</t>
   </si>
   <si>
-    <t>20250529111700</t>
+    <t>Settle Petty Expense</t>
+  </si>
+  <si>
+    <t>icon:images/action_button.gif
+dialog:content: Are you sure to settle this petty expense?</t>
+  </si>
+  <si>
+    <t>bttSettlePettyExpense</t>
+  </si>
+  <si>
+    <t>20250603115800</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1443,7 +1442,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1489,6 +1488,9 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,6 +1506,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1630,6 +1637,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1664,6 +1672,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1839,7 +1848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T195"/>
   <sheetViews>
@@ -1847,7 +1856,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1874,7 +1883,7 @@
     <col min="29" max="31" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="37.5" customHeight="1">
+    <row r="1" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1883,10 +1892,10 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1897,7 +1906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1919,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +1932,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +1947,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1953,7 +1962,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1966,7 +1975,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
@@ -1979,7 +1988,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -1992,7 +2001,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2029,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -2033,7 +2042,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
@@ -2048,7 +2057,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -2059,13 +2068,13 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="I16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="C17" s="9" t="s">
         <v>40</v>
@@ -2079,7 +2088,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="C19" s="11" t="s">
         <v>50</v>
@@ -2124,7 +2133,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
         <v>53</v>
       </c>
@@ -2139,7 +2148,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="11" t="s">
         <v>55</v>
       </c>
@@ -2154,7 +2163,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" s="11" t="s">
         <v>57</v>
       </c>
@@ -2169,7 +2178,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
         <v>58</v>
       </c>
@@ -2184,7 +2193,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C24" s="11" t="s">
         <v>60</v>
       </c>
@@ -2199,7 +2208,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" s="11" t="s">
         <v>61</v>
       </c>
@@ -2214,7 +2223,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26" s="11" t="s">
         <v>62</v>
       </c>
@@ -2231,7 +2240,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>66</v>
       </c>
@@ -2246,7 +2255,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="C28" s="5" t="s">
         <v>68</v>
@@ -2258,10 +2267,10 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="D30" s="9" t="s">
         <v>69</v>
@@ -2270,7 +2279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
@@ -2300,7 +2309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>76</v>
       </c>
@@ -2362,7 +2371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="11" t="s">
         <v>93</v>
@@ -2393,7 +2402,7 @@
       <c r="S33" s="11"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C34" s="11" t="s">
         <v>95</v>
       </c>
@@ -2419,7 +2428,7 @@
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="2:20">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
         <v>98</v>
       </c>
@@ -2453,7 +2462,7 @@
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="2:20">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C36" s="11" t="s">
         <v>102</v>
       </c>
@@ -2481,7 +2490,7 @@
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>
     </row>
-    <row r="37" spans="2:20">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C37" s="11" t="s">
         <v>105</v>
       </c>
@@ -2511,7 +2520,7 @@
       <c r="S37" s="11"/>
       <c r="T37" s="11"/>
     </row>
-    <row r="38" spans="2:20">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
         <v>108</v>
       </c>
@@ -2539,7 +2548,7 @@
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
     </row>
-    <row r="39" spans="2:20">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C39" s="11" t="s">
         <v>110</v>
       </c>
@@ -2565,7 +2574,7 @@
       <c r="S39" s="11"/>
       <c r="T39" s="11"/>
     </row>
-    <row r="40" spans="2:20">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C40" s="11" t="s">
         <v>111</v>
       </c>
@@ -2595,7 +2604,7 @@
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
     </row>
-    <row r="41" spans="2:20">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C41" s="11" t="s">
         <v>113</v>
       </c>
@@ -2625,7 +2634,7 @@
       <c r="S41" s="11"/>
       <c r="T41" s="11"/>
     </row>
-    <row r="42" spans="2:20">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C42" s="11" t="s">
         <v>115</v>
       </c>
@@ -2657,7 +2666,7 @@
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
     </row>
-    <row r="43" spans="2:20">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C43" s="11" t="s">
         <v>117</v>
       </c>
@@ -2683,7 +2692,7 @@
       <c r="S43" s="11"/>
       <c r="T43" s="11"/>
     </row>
-    <row r="44" spans="2:20">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C44" s="11" t="s">
         <v>119</v>
       </c>
@@ -2709,7 +2718,7 @@
       <c r="S44" s="11"/>
       <c r="T44" s="11"/>
     </row>
-    <row r="45" spans="2:20">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
         <v>120</v>
       </c>
@@ -2737,7 +2746,7 @@
       <c r="S45" s="11"/>
       <c r="T45" s="11"/>
     </row>
-    <row r="46" spans="2:20">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
         <v>68</v>
       </c>
@@ -2759,11 +2768,11 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="48" spans="2:20">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="K48" s="9"/>
       <c r="M48" s="9"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
         <v>122</v>
@@ -2785,7 +2794,7 @@
       </c>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>126</v>
       </c>
@@ -2835,7 +2844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="11" t="s">
         <v>93</v>
@@ -2862,7 +2871,7 @@
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C52" s="11"/>
       <c r="D52" s="11" t="s">
         <v>141</v>
@@ -2884,7 +2893,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C53" s="11"/>
       <c r="D53" s="11" t="s">
         <v>143</v>
@@ -2910,7 +2919,7 @@
       </c>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
         <v>148</v>
@@ -2932,7 +2941,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C55" s="11"/>
       <c r="D55" s="11" t="s">
         <v>150</v>
@@ -2954,7 +2963,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C56" s="11"/>
       <c r="D56" s="11" t="s">
         <v>152</v>
@@ -2976,7 +2985,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C57" s="11"/>
       <c r="D57" s="11" t="s">
         <v>154</v>
@@ -2998,7 +3007,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
         <v>156</v>
@@ -3020,7 +3029,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C59" s="11"/>
       <c r="D59" s="11" t="s">
         <v>158</v>
@@ -3042,7 +3051,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" s="11"/>
       <c r="D60" s="11" t="s">
         <v>160</v>
@@ -3066,7 +3075,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C61" s="11"/>
       <c r="D61" s="11" t="s">
         <v>164</v>
@@ -3090,7 +3099,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" s="11"/>
       <c r="D62" s="11" t="s">
         <v>166</v>
@@ -3114,7 +3123,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C63" s="11"/>
       <c r="D63" s="11" t="s">
         <v>168</v>
@@ -3138,7 +3147,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C64" s="11"/>
       <c r="D64" s="11" t="s">
         <v>170</v>
@@ -3162,7 +3171,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="3:16">
+    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C65" s="11"/>
       <c r="D65" s="11" t="s">
         <v>172</v>
@@ -3186,7 +3195,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="3:16">
+    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C66" s="11"/>
       <c r="D66" s="11" t="s">
         <v>174</v>
@@ -3208,7 +3217,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="3:16">
+    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C67" s="11"/>
       <c r="D67" s="11" t="s">
         <v>176</v>
@@ -3230,7 +3239,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="68" spans="3:16">
+    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C68" s="11"/>
       <c r="D68" s="11" t="s">
         <v>178</v>
@@ -3252,7 +3261,7 @@
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
     </row>
-    <row r="69" spans="3:16">
+    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C69" s="11" t="s">
         <v>98</v>
       </c>
@@ -3278,7 +3287,7 @@
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
     </row>
-    <row r="70" spans="3:16">
+    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
         <v>182</v>
@@ -3304,7 +3313,7 @@
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
     </row>
-    <row r="71" spans="3:16">
+    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C71" s="11"/>
       <c r="D71" s="11" t="s">
         <v>186</v>
@@ -3328,7 +3337,7 @@
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
     </row>
-    <row r="72" spans="3:16">
+    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
         <v>189</v>
@@ -3354,7 +3363,7 @@
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
     </row>
-    <row r="73" spans="3:16">
+    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C73" s="11"/>
       <c r="D73" s="11" t="s">
         <v>192</v>
@@ -3378,7 +3387,7 @@
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
     </row>
-    <row r="74" spans="3:16">
+    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C74" s="11"/>
       <c r="D74" s="11" t="s">
         <v>194</v>
@@ -3402,7 +3411,7 @@
       <c r="O74" s="11"/>
       <c r="P74" s="11"/>
     </row>
-    <row r="75" spans="3:16">
+    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
         <v>197</v>
@@ -3428,7 +3437,7 @@
       <c r="O75" s="11"/>
       <c r="P75" s="11"/>
     </row>
-    <row r="76" spans="3:16">
+    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C76" s="11"/>
       <c r="D76" s="11" t="s">
         <v>201</v>
@@ -3452,7 +3461,7 @@
       <c r="O76" s="11"/>
       <c r="P76" s="11"/>
     </row>
-    <row r="77" spans="3:16">
+    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C77" s="11"/>
       <c r="D77" s="11" t="s">
         <v>204</v>
@@ -3476,7 +3485,7 @@
       <c r="O77" s="11"/>
       <c r="P77" s="11"/>
     </row>
-    <row r="78" spans="3:16">
+    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
         <v>206</v>
@@ -3502,7 +3511,7 @@
       <c r="O78" s="11"/>
       <c r="P78" s="11"/>
     </row>
-    <row r="79" spans="3:16">
+    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C79" s="11"/>
       <c r="D79" s="11" t="s">
         <v>209</v>
@@ -3526,7 +3535,7 @@
       <c r="O79" s="11"/>
       <c r="P79" s="11"/>
     </row>
-    <row r="80" spans="3:16">
+    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C80" s="11"/>
       <c r="D80" s="11" t="s">
         <v>212</v>
@@ -3550,7 +3559,7 @@
       <c r="O80" s="11"/>
       <c r="P80" s="11"/>
     </row>
-    <row r="81" spans="3:16">
+    <row r="81" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C81" s="11"/>
       <c r="D81" s="11" t="s">
         <v>214</v>
@@ -3574,7 +3583,7 @@
       <c r="O81" s="11"/>
       <c r="P81" s="11"/>
     </row>
-    <row r="82" spans="3:16">
+    <row r="82" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C82" s="11"/>
       <c r="D82" s="11" t="s">
         <v>217</v>
@@ -3598,7 +3607,7 @@
       <c r="O82" s="11"/>
       <c r="P82" s="11"/>
     </row>
-    <row r="83" spans="3:16">
+    <row r="83" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C83" s="11" t="s">
         <v>105</v>
       </c>
@@ -3624,7 +3633,7 @@
       <c r="O83" s="11"/>
       <c r="P83" s="11"/>
     </row>
-    <row r="84" spans="3:16">
+    <row r="84" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C84" s="11"/>
       <c r="D84" s="11" t="s">
         <v>224</v>
@@ -3650,7 +3659,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="3:16">
+    <row r="85" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C85" s="11"/>
       <c r="D85" s="11" t="s">
         <v>227</v>
@@ -3674,7 +3683,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="3:16">
+    <row r="86" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C86" s="11"/>
       <c r="D86" s="11" t="s">
         <v>229</v>
@@ -3698,7 +3707,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="3:16">
+    <row r="87" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C87" s="11"/>
       <c r="D87" s="11" t="s">
         <v>231</v>
@@ -3722,7 +3731,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="3:16">
+    <row r="88" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C88" s="11"/>
       <c r="D88" s="11" t="s">
         <v>234</v>
@@ -3746,7 +3755,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="3:16">
+    <row r="89" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C89" s="11"/>
       <c r="D89" s="11" t="s">
         <v>237</v>
@@ -3770,7 +3779,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="3:16">
+    <row r="90" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C90" s="11"/>
       <c r="D90" s="11" t="s">
         <v>240</v>
@@ -3794,7 +3803,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="3:16">
+    <row r="91" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C91" s="11"/>
       <c r="D91" s="11" t="s">
         <v>243</v>
@@ -3820,7 +3829,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="3:16">
+    <row r="92" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C92" s="11"/>
       <c r="D92" s="11" t="s">
         <v>246</v>
@@ -3844,7 +3853,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="3:16">
+    <row r="93" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C93" s="11"/>
       <c r="D93" s="11" t="s">
         <v>248</v>
@@ -3870,7 +3879,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="3:16">
+    <row r="94" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C94" s="11"/>
       <c r="D94" s="11" t="s">
         <v>253</v>
@@ -3896,7 +3905,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="3:16">
+    <row r="95" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C95" s="11" t="s">
         <v>108</v>
       </c>
@@ -3922,7 +3931,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="3:16">
+    <row r="96" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
@@ -3948,7 +3957,7 @@
       </c>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="3:16">
+    <row r="97" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11" t="s">
@@ -3974,7 +3983,7 @@
       </c>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="3:16">
+    <row r="98" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11" t="s">
@@ -4000,7 +4009,7 @@
       </c>
       <c r="P98" s="11"/>
     </row>
-    <row r="99" spans="3:16">
+    <row r="99" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11" t="s">
@@ -4026,7 +4035,7 @@
       </c>
       <c r="P99" s="11"/>
     </row>
-    <row r="100" spans="3:16">
+    <row r="100" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11" t="s">
@@ -4054,7 +4063,7 @@
       </c>
       <c r="P100" s="11"/>
     </row>
-    <row r="101" spans="3:16">
+    <row r="101" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
@@ -4078,7 +4087,7 @@
       <c r="O101" s="11"/>
       <c r="P101" s="11"/>
     </row>
-    <row r="102" spans="3:16">
+    <row r="102" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
@@ -4104,7 +4113,7 @@
       </c>
       <c r="P102" s="11"/>
     </row>
-    <row r="103" spans="3:16">
+    <row r="103" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11" t="s">
@@ -4130,7 +4139,7 @@
       </c>
       <c r="P103" s="11"/>
     </row>
-    <row r="104" spans="3:16">
+    <row r="104" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11" t="s">
@@ -4156,7 +4165,7 @@
       </c>
       <c r="P104" s="11"/>
     </row>
-    <row r="105" spans="3:16">
+    <row r="105" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11" t="s">
@@ -4182,7 +4191,7 @@
       </c>
       <c r="P105" s="11"/>
     </row>
-    <row r="106" spans="3:16">
+    <row r="106" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C106" s="11"/>
       <c r="D106" s="11" t="s">
         <v>270</v>
@@ -4210,7 +4219,7 @@
       </c>
       <c r="P106" s="11"/>
     </row>
-    <row r="107" spans="3:16">
+    <row r="107" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C107" s="11"/>
       <c r="D107" s="11" t="s">
         <v>274</v>
@@ -4236,7 +4245,7 @@
       </c>
       <c r="P107" s="11"/>
     </row>
-    <row r="108" spans="3:16">
+    <row r="108" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11" t="s">
@@ -4264,7 +4273,7 @@
       </c>
       <c r="P108" s="11"/>
     </row>
-    <row r="109" spans="3:16">
+    <row r="109" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C109" s="11"/>
       <c r="D109" s="11" t="s">
         <v>279</v>
@@ -4290,7 +4299,7 @@
       </c>
       <c r="P109" s="11"/>
     </row>
-    <row r="110" spans="3:16">
+    <row r="110" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C110" s="11"/>
       <c r="D110" s="11" t="s">
         <v>282</v>
@@ -4316,7 +4325,7 @@
       </c>
       <c r="P110" s="11"/>
     </row>
-    <row r="111" spans="3:16">
+    <row r="111" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C111" s="11" t="s">
         <v>110</v>
       </c>
@@ -4342,7 +4351,7 @@
       <c r="O111" s="11"/>
       <c r="P111" s="11"/>
     </row>
-    <row r="112" spans="3:16">
+    <row r="112" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C112" s="11" t="s">
         <v>111</v>
       </c>
@@ -4368,7 +4377,7 @@
       <c r="O112" s="11"/>
       <c r="P112" s="11"/>
     </row>
-    <row r="113" spans="3:16">
+    <row r="113" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C113" s="11"/>
       <c r="D113" s="11" t="s">
         <v>291</v>
@@ -4392,7 +4401,7 @@
       <c r="O113" s="11"/>
       <c r="P113" s="11"/>
     </row>
-    <row r="114" spans="3:16">
+    <row r="114" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C114" s="11"/>
       <c r="D114" s="11" t="s">
         <v>294</v>
@@ -4416,7 +4425,7 @@
       <c r="O114" s="11"/>
       <c r="P114" s="11"/>
     </row>
-    <row r="115" spans="3:16">
+    <row r="115" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C115" s="11"/>
       <c r="D115" s="11" t="s">
         <v>296</v>
@@ -4440,7 +4449,7 @@
       <c r="O115" s="11"/>
       <c r="P115" s="11"/>
     </row>
-    <row r="116" spans="3:16">
+    <row r="116" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C116" s="11"/>
       <c r="D116" s="11" t="s">
         <v>299</v>
@@ -4464,7 +4473,7 @@
       <c r="O116" s="11"/>
       <c r="P116" s="11"/>
     </row>
-    <row r="117" spans="3:16">
+    <row r="117" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C117" s="11"/>
       <c r="D117" s="11" t="s">
         <v>301</v>
@@ -4488,7 +4497,7 @@
       <c r="O117" s="11"/>
       <c r="P117" s="11"/>
     </row>
-    <row r="118" spans="3:16">
+    <row r="118" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C118" s="11"/>
       <c r="D118" s="11" t="s">
         <v>304</v>
@@ -4512,7 +4521,7 @@
       <c r="O118" s="11"/>
       <c r="P118" s="11"/>
     </row>
-    <row r="119" spans="3:16">
+    <row r="119" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C119" s="11"/>
       <c r="D119" s="11" t="s">
         <v>307</v>
@@ -4536,7 +4545,7 @@
       <c r="O119" s="11"/>
       <c r="P119" s="11"/>
     </row>
-    <row r="120" spans="3:16">
+    <row r="120" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C120" s="11" t="s">
         <v>113</v>
       </c>
@@ -4564,7 +4573,7 @@
       <c r="O120" s="11"/>
       <c r="P120" s="11"/>
     </row>
-    <row r="121" spans="3:16">
+    <row r="121" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C121" s="11"/>
       <c r="D121" s="11" t="s">
         <v>291</v>
@@ -4590,7 +4599,7 @@
       <c r="O121" s="11"/>
       <c r="P121" s="11"/>
     </row>
-    <row r="122" spans="3:16">
+    <row r="122" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C122" s="11"/>
       <c r="D122" s="11" t="s">
         <v>314</v>
@@ -4616,7 +4625,7 @@
       <c r="O122" s="11"/>
       <c r="P122" s="11"/>
     </row>
-    <row r="123" spans="3:16">
+    <row r="123" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C123" s="11"/>
       <c r="D123" s="11" t="s">
         <v>307</v>
@@ -4642,7 +4651,7 @@
       <c r="O123" s="11"/>
       <c r="P123" s="11"/>
     </row>
-    <row r="124" spans="3:16">
+    <row r="124" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C124" s="11" t="s">
         <v>115</v>
       </c>
@@ -4672,7 +4681,7 @@
       <c r="O124" s="11"/>
       <c r="P124" s="11"/>
     </row>
-    <row r="125" spans="3:16">
+    <row r="125" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C125" s="11"/>
       <c r="D125" s="11" t="s">
         <v>321</v>
@@ -4698,7 +4707,7 @@
       <c r="O125" s="11"/>
       <c r="P125" s="11"/>
     </row>
-    <row r="126" spans="3:16">
+    <row r="126" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C126" s="11"/>
       <c r="D126" s="11" t="s">
         <v>322</v>
@@ -4726,7 +4735,7 @@
       <c r="O126" s="11"/>
       <c r="P126" s="11"/>
     </row>
-    <row r="127" spans="3:16">
+    <row r="127" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C127" s="11"/>
       <c r="D127" s="11" t="s">
         <v>325</v>
@@ -4754,7 +4763,7 @@
       <c r="O127" s="11"/>
       <c r="P127" s="11"/>
     </row>
-    <row r="128" spans="3:16">
+    <row r="128" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C128" s="11"/>
       <c r="D128" s="11" t="s">
         <v>328</v>
@@ -4780,7 +4789,7 @@
       <c r="O128" s="11"/>
       <c r="P128" s="11"/>
     </row>
-    <row r="129" spans="3:16">
+    <row r="129" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C129" s="11" t="s">
         <v>117</v>
       </c>
@@ -4808,7 +4817,7 @@
       <c r="O129" s="11"/>
       <c r="P129" s="11"/>
     </row>
-    <row r="130" spans="3:16">
+    <row r="130" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C130" s="11"/>
       <c r="D130" s="11" t="s">
         <v>337</v>
@@ -4834,7 +4843,7 @@
       <c r="O130" s="11"/>
       <c r="P130" s="11"/>
     </row>
-    <row r="131" spans="3:16">
+    <row r="131" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C131" s="11"/>
       <c r="D131" s="11" t="s">
         <v>341</v>
@@ -4860,7 +4869,7 @@
       <c r="O131" s="11"/>
       <c r="P131" s="11"/>
     </row>
-    <row r="132" spans="3:16">
+    <row r="132" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C132" s="11"/>
       <c r="D132" s="11" t="s">
         <v>345</v>
@@ -4886,7 +4895,7 @@
       <c r="O132" s="11"/>
       <c r="P132" s="11"/>
     </row>
-    <row r="133" spans="3:16">
+    <row r="133" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C133" s="11" t="s">
         <v>119</v>
       </c>
@@ -4914,7 +4923,7 @@
       <c r="O133" s="11"/>
       <c r="P133" s="11"/>
     </row>
-    <row r="134" spans="3:16">
+    <row r="134" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C134" s="11"/>
       <c r="D134" s="11" t="s">
         <v>353</v>
@@ -4940,7 +4949,7 @@
       <c r="O134" s="11"/>
       <c r="P134" s="11"/>
     </row>
-    <row r="135" spans="3:16">
+    <row r="135" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C135" s="11"/>
       <c r="D135" s="11" t="s">
         <v>357</v>
@@ -4966,7 +4975,7 @@
       <c r="O135" s="11"/>
       <c r="P135" s="11"/>
     </row>
-    <row r="136" spans="3:16">
+    <row r="136" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C136" s="11"/>
       <c r="D136" s="11" t="s">
         <v>361</v>
@@ -4992,13 +5001,13 @@
       <c r="O136" s="11"/>
       <c r="P136" s="11"/>
     </row>
-    <row r="137" spans="3:16">
+    <row r="137" spans="3:16" ht="75" x14ac:dyDescent="0.25">
       <c r="C137" s="11"/>
       <c r="D137" s="11" t="s">
-        <v>365</v>
+        <v>412</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="F137" s="11"/>
       <c r="G137" s="11"/>
@@ -5008,23 +5017,23 @@
       <c r="K137" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="L137" s="11" t="s">
-        <v>367</v>
+      <c r="L137" s="19" t="s">
+        <v>411</v>
       </c>
       <c r="M137" s="11"/>
       <c r="N137" s="11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="O137" s="11"/>
       <c r="P137" s="11"/>
     </row>
-    <row r="138" spans="3:16">
+    <row r="138" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C138" s="11"/>
       <c r="D138" s="11" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F138" s="11"/>
       <c r="G138" s="11"/>
@@ -5035,22 +5044,22 @@
         <v>334</v>
       </c>
       <c r="L138" s="11" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="M138" s="11"/>
       <c r="N138" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="O138" s="11"/>
       <c r="P138" s="11"/>
     </row>
-    <row r="139" spans="3:16">
+    <row r="139" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C139" s="11"/>
       <c r="D139" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F139" s="11"/>
       <c r="G139" s="11"/>
@@ -5065,18 +5074,18 @@
       </c>
       <c r="M139" s="11"/>
       <c r="N139" s="11" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="O139" s="11"/>
       <c r="P139" s="11"/>
     </row>
-    <row r="140" spans="3:16">
+    <row r="140" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C140" s="11"/>
       <c r="D140" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F140" s="11"/>
       <c r="G140" s="11"/>
@@ -5091,18 +5100,18 @@
       </c>
       <c r="M140" s="11"/>
       <c r="N140" s="11" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="O140" s="11"/>
       <c r="P140" s="11"/>
     </row>
-    <row r="141" spans="3:16">
+    <row r="141" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C141" s="11"/>
       <c r="D141" s="11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E141" s="11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F141" s="11"/>
       <c r="G141" s="11"/>
@@ -5113,22 +5122,22 @@
         <v>334</v>
       </c>
       <c r="L141" s="11" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="M141" s="11"/>
       <c r="N141" s="11" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O141" s="11"/>
       <c r="P141" s="11"/>
     </row>
-    <row r="142" spans="3:16">
+    <row r="142" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C142" s="11"/>
       <c r="D142" s="11" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E142" s="11" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F142" s="11"/>
       <c r="G142" s="11"/>
@@ -5139,16 +5148,16 @@
         <v>334</v>
       </c>
       <c r="L142" s="11" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="M142" s="11"/>
       <c r="N142" s="11" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
     </row>
-    <row r="143" spans="3:16">
+    <row r="143" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C143" s="11" t="s">
         <v>120</v>
       </c>
@@ -5166,17 +5175,17 @@
       <c r="K143" s="11"/>
       <c r="L143" s="11"/>
       <c r="M143" s="11" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N143" s="11"/>
       <c r="O143" s="11"/>
       <c r="P143" s="11"/>
     </row>
-    <row r="144" spans="3:16">
+    <row r="144" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F144" s="11"/>
       <c r="G144" s="11"/>
@@ -5188,13 +5197,13 @@
       <c r="K144" s="11"/>
       <c r="L144" s="11"/>
       <c r="M144" s="11" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="N144" s="11"/>
       <c r="O144" s="11"/>
       <c r="P144" s="11"/>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C145" s="11"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11" t="s">
@@ -5216,7 +5225,7 @@
       <c r="O145" s="11"/>
       <c r="P145" s="11"/>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C146" s="11"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11" t="s">
@@ -5238,7 +5247,7 @@
       <c r="O146" s="11"/>
       <c r="P146" s="11"/>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C147" s="5" t="s">
         <v>68</v>
       </c>
@@ -5256,15 +5265,15 @@
       <c r="O147" s="3"/>
       <c r="P147" s="3"/>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>77</v>
@@ -5273,52 +5282,52 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C153" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
       <c r="G158" s="11"/>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C159" s="5" t="s">
         <v>68</v>
       </c>
@@ -5327,17 +5336,17 @@
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B162" s="16" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B163" s="13"/>
       <c r="C163" s="17" t="s">
@@ -5347,25 +5356,25 @@
         <v>135</v>
       </c>
       <c r="E163" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="F163" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="G163" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="H163" s="17" t="s">
         <v>401</v>
-      </c>
-      <c r="F163" s="17" t="s">
-        <v>402</v>
-      </c>
-      <c r="G163" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="H163" s="17" t="s">
-        <v>404</v>
       </c>
       <c r="I163" s="17" t="s">
         <v>39</v>
       </c>
       <c r="K163" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C164" s="11" t="s">
         <v>98</v>
       </c>
@@ -5380,10 +5389,10 @@
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
       <c r="K164" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C165" s="11"/>
       <c r="D165" s="11" t="s">
         <v>182</v>
@@ -5396,7 +5405,7 @@
       <c r="H165" s="11"/>
       <c r="I165" s="11"/>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C166" s="11"/>
       <c r="D166" s="11" t="s">
         <v>186</v>
@@ -5409,7 +5418,7 @@
       <c r="H166" s="11"/>
       <c r="I166" s="11"/>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C167" s="11"/>
       <c r="D167" s="11" t="s">
         <v>189</v>
@@ -5422,7 +5431,7 @@
       <c r="H167" s="11"/>
       <c r="I167" s="11"/>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C168" s="11"/>
       <c r="D168" s="11" t="s">
         <v>192</v>
@@ -5435,7 +5444,7 @@
       <c r="H168" s="11"/>
       <c r="I168" s="11"/>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C169" s="11"/>
       <c r="D169" s="11" t="s">
         <v>194</v>
@@ -5450,7 +5459,7 @@
       <c r="H169" s="11"/>
       <c r="I169" s="11"/>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C170" s="11"/>
       <c r="D170" s="11" t="s">
         <v>197</v>
@@ -5463,7 +5472,7 @@
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C171" s="11"/>
       <c r="D171" s="11" t="s">
         <v>201</v>
@@ -5476,13 +5485,13 @@
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C172" s="11"/>
       <c r="D172" s="11" t="s">
         <v>204</v>
       </c>
       <c r="E172" s="11" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F172" s="11" t="s">
         <v>144</v>
@@ -5491,7 +5500,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="11"/>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C173" s="11"/>
       <c r="D173" s="11" t="s">
         <v>206</v>
@@ -5504,7 +5513,7 @@
       <c r="H173" s="11"/>
       <c r="I173" s="11"/>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C174" s="11"/>
       <c r="D174" s="11" t="s">
         <v>209</v>
@@ -5519,7 +5528,7 @@
       <c r="H174" s="11"/>
       <c r="I174" s="11"/>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C175" s="11"/>
       <c r="D175" s="11" t="s">
         <v>212</v>
@@ -5532,20 +5541,20 @@
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C176" s="11"/>
       <c r="D176" s="11" t="s">
         <v>214</v>
       </c>
       <c r="E176" s="11" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F176" s="11"/>
       <c r="G176" s="11"/>
       <c r="H176" s="11"/>
       <c r="I176" s="11"/>
     </row>
-    <row r="177" spans="3:9">
+    <row r="177" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C177" s="11" t="s">
         <v>111</v>
       </c>
@@ -5560,7 +5569,7 @@
       <c r="H177" s="11"/>
       <c r="I177" s="11"/>
     </row>
-    <row r="178" spans="3:9">
+    <row r="178" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C178" s="11"/>
       <c r="D178" s="11" t="s">
         <v>291</v>
@@ -5573,7 +5582,7 @@
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
     </row>
-    <row r="179" spans="3:9">
+    <row r="179" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
         <v>294</v>
@@ -5586,7 +5595,7 @@
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
     </row>
-    <row r="180" spans="3:9">
+    <row r="180" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
         <v>296</v>
@@ -5597,11 +5606,11 @@
       <c r="F180" s="11"/>
       <c r="G180" s="11"/>
       <c r="H180" s="11" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I180" s="11"/>
     </row>
-    <row r="181" spans="3:9">
+    <row r="181" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C181" s="11"/>
       <c r="D181" s="11" t="s">
         <v>299</v>
@@ -5612,11 +5621,11 @@
       <c r="F181" s="11"/>
       <c r="G181" s="11"/>
       <c r="H181" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I181" s="11"/>
     </row>
-    <row r="182" spans="3:9">
+    <row r="182" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
         <v>301</v>
@@ -5627,11 +5636,11 @@
       <c r="F182" s="11"/>
       <c r="G182" s="11"/>
       <c r="H182" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I182" s="11"/>
     </row>
-    <row r="183" spans="3:9">
+    <row r="183" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C183" s="11"/>
       <c r="D183" s="11" t="s">
         <v>304</v>
@@ -5642,11 +5651,11 @@
       <c r="F183" s="11"/>
       <c r="G183" s="11"/>
       <c r="H183" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I183" s="11"/>
     </row>
-    <row r="184" spans="3:9">
+    <row r="184" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
         <v>307</v>
@@ -5657,11 +5666,11 @@
       <c r="F184" s="11"/>
       <c r="G184" s="11"/>
       <c r="H184" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I184" s="11"/>
     </row>
-    <row r="185" spans="3:9">
+    <row r="185" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C185" s="11" t="s">
         <v>113</v>
       </c>
@@ -5676,7 +5685,7 @@
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
     </row>
-    <row r="186" spans="3:9">
+    <row r="186" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
         <v>291</v>
@@ -5689,7 +5698,7 @@
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
     </row>
-    <row r="187" spans="3:9">
+    <row r="187" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
         <v>314</v>
@@ -5700,11 +5709,11 @@
       <c r="F187" s="11"/>
       <c r="G187" s="11"/>
       <c r="H187" s="11" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I187" s="11"/>
     </row>
-    <row r="188" spans="3:9">
+    <row r="188" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C188" s="11"/>
       <c r="D188" s="11" t="s">
         <v>307</v>
@@ -5715,11 +5724,11 @@
       <c r="F188" s="11"/>
       <c r="G188" s="11"/>
       <c r="H188" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I188" s="11"/>
     </row>
-    <row r="189" spans="3:9">
+    <row r="189" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C189" s="11" t="s">
         <v>115</v>
       </c>
@@ -5734,7 +5743,7 @@
       <c r="H189" s="11"/>
       <c r="I189" s="11"/>
     </row>
-    <row r="190" spans="3:9">
+    <row r="190" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C190" s="11"/>
       <c r="D190" s="11" t="s">
         <v>321</v>
@@ -5745,11 +5754,11 @@
       <c r="F190" s="11"/>
       <c r="G190" s="11"/>
       <c r="H190" s="11" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I190" s="11"/>
     </row>
-    <row r="191" spans="3:9">
+    <row r="191" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
         <v>322</v>
@@ -5760,11 +5769,11 @@
       <c r="F191" s="11"/>
       <c r="G191" s="11"/>
       <c r="H191" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I191" s="11"/>
     </row>
-    <row r="192" spans="3:9">
+    <row r="192" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
         <v>325</v>
@@ -5775,11 +5784,11 @@
       <c r="F192" s="11"/>
       <c r="G192" s="11"/>
       <c r="H192" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I192" s="11"/>
     </row>
-    <row r="193" spans="3:9">
+    <row r="193" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
         <v>328</v>
@@ -5790,11 +5799,11 @@
       <c r="F193" s="11"/>
       <c r="G193" s="11"/>
       <c r="H193" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I193" s="11"/>
     </row>
-    <row r="194" spans="3:9">
+    <row r="194" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C194" s="5" t="s">
         <v>68</v>
       </c>
@@ -5805,7 +5814,7 @@
       <c r="H194" s="3"/>
       <c r="I194" s="3"/>
     </row>
-    <row r="195" spans="3:9">
+    <row r="195" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H195" s="8"/>
     </row>
   </sheetData>
@@ -5816,20 +5825,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A5:C32"/>
   <sheetViews>
@@ -5837,25 +5846,25 @@
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>